<commit_message>
Atualização da Documentação - LN e ODS
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Mapeamento ODS_LN.xlsx
+++ b/Documentação/Planilhas/Mapeamento ODS_LN.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="338">
   <si>
     <t>TABELA</t>
   </si>
@@ -1027,6 +1027,9 @@
   </si>
   <si>
     <t>NR_RECEB_DOCTO_WMS</t>
+  </si>
+  <si>
+    <t>SQ_ORDEM</t>
   </si>
 </sst>
 </file>
@@ -1079,11 +1082,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:D593" totalsRowShown="0">
-  <autoFilter ref="A1:D593">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:D595" totalsRowShown="0">
+  <autoFilter ref="A1:D595">
     <filterColumn colId="0">
       <filters>
-        <filter val="ln.ods_nfr_cab"/>
+        <filter val="ln.ods_pev_det"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -1382,10 +1385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D593"/>
+  <dimension ref="A1:D595"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A197" workbookViewId="0">
-      <selection activeCell="C594" sqref="C594"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A540" workbookViewId="0">
+      <selection activeCell="C560" sqref="C560"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3200,7 +3203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:4">
+    <row r="155" spans="1:4" hidden="1">
       <c r="A155" t="s">
         <v>132</v>
       </c>
@@ -3211,7 +3214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:4">
+    <row r="156" spans="1:4" hidden="1">
       <c r="A156" t="s">
         <v>132</v>
       </c>
@@ -3222,7 +3225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:4">
+    <row r="157" spans="1:4" hidden="1">
       <c r="A157" t="s">
         <v>132</v>
       </c>
@@ -3233,7 +3236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:4">
+    <row r="158" spans="1:4" hidden="1">
       <c r="A158" t="s">
         <v>132</v>
       </c>
@@ -3244,7 +3247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:4">
+    <row r="159" spans="1:4" hidden="1">
       <c r="A159" t="s">
         <v>132</v>
       </c>
@@ -3255,7 +3258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:4">
+    <row r="160" spans="1:4" hidden="1">
       <c r="A160" t="s">
         <v>132</v>
       </c>
@@ -3266,7 +3269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:4">
+    <row r="161" spans="1:4" hidden="1">
       <c r="A161" t="s">
         <v>132</v>
       </c>
@@ -3280,7 +3283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:4">
+    <row r="162" spans="1:4" hidden="1">
       <c r="A162" t="s">
         <v>132</v>
       </c>
@@ -3294,7 +3297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:4">
+    <row r="163" spans="1:4" hidden="1">
       <c r="A163" t="s">
         <v>132</v>
       </c>
@@ -3308,7 +3311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:4">
+    <row r="164" spans="1:4" hidden="1">
       <c r="A164" t="s">
         <v>132</v>
       </c>
@@ -3322,7 +3325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:4">
+    <row r="165" spans="1:4" hidden="1">
       <c r="A165" t="s">
         <v>132</v>
       </c>
@@ -3336,7 +3339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:4">
+    <row r="166" spans="1:4" hidden="1">
       <c r="A166" t="s">
         <v>132</v>
       </c>
@@ -3347,7 +3350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:4">
+    <row r="167" spans="1:4" hidden="1">
       <c r="A167" t="s">
         <v>132</v>
       </c>
@@ -3358,7 +3361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:4">
+    <row r="168" spans="1:4" hidden="1">
       <c r="A168" t="s">
         <v>132</v>
       </c>
@@ -3369,7 +3372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:4">
+    <row r="169" spans="1:4" hidden="1">
       <c r="A169" t="s">
         <v>132</v>
       </c>
@@ -3380,7 +3383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:4">
+    <row r="170" spans="1:4" hidden="1">
       <c r="A170" t="s">
         <v>132</v>
       </c>
@@ -3391,7 +3394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:4">
+    <row r="171" spans="1:4" hidden="1">
       <c r="A171" t="s">
         <v>132</v>
       </c>
@@ -3405,7 +3408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:4">
+    <row r="172" spans="1:4" hidden="1">
       <c r="A172" t="s">
         <v>132</v>
       </c>
@@ -3419,7 +3422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:4">
+    <row r="173" spans="1:4" hidden="1">
       <c r="A173" t="s">
         <v>132</v>
       </c>
@@ -3433,7 +3436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:4">
+    <row r="174" spans="1:4" hidden="1">
       <c r="A174" t="s">
         <v>132</v>
       </c>
@@ -3447,7 +3450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:4">
+    <row r="175" spans="1:4" hidden="1">
       <c r="A175" t="s">
         <v>132</v>
       </c>
@@ -3461,7 +3464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:4">
+    <row r="176" spans="1:4" hidden="1">
       <c r="A176" t="s">
         <v>132</v>
       </c>
@@ -3475,7 +3478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:4">
+    <row r="177" spans="1:4" hidden="1">
       <c r="A177" t="s">
         <v>132</v>
       </c>
@@ -3489,7 +3492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:4">
+    <row r="178" spans="1:4" hidden="1">
       <c r="A178" t="s">
         <v>132</v>
       </c>
@@ -3503,7 +3506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:4">
+    <row r="179" spans="1:4" hidden="1">
       <c r="A179" t="s">
         <v>132</v>
       </c>
@@ -3517,7 +3520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:4">
+    <row r="180" spans="1:4" hidden="1">
       <c r="A180" t="s">
         <v>132</v>
       </c>
@@ -3531,7 +3534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:4">
+    <row r="181" spans="1:4" hidden="1">
       <c r="A181" t="s">
         <v>132</v>
       </c>
@@ -3545,7 +3548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:4">
+    <row r="182" spans="1:4" hidden="1">
       <c r="A182" t="s">
         <v>132</v>
       </c>
@@ -3559,7 +3562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:4">
+    <row r="183" spans="1:4" hidden="1">
       <c r="A183" t="s">
         <v>132</v>
       </c>
@@ -3573,7 +3576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:4">
+    <row r="184" spans="1:4" hidden="1">
       <c r="A184" t="s">
         <v>132</v>
       </c>
@@ -3587,7 +3590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:4">
+    <row r="185" spans="1:4" hidden="1">
       <c r="A185" t="s">
         <v>132</v>
       </c>
@@ -3601,7 +3604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:4">
+    <row r="186" spans="1:4" hidden="1">
       <c r="A186" t="s">
         <v>132</v>
       </c>
@@ -3612,7 +3615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:4">
+    <row r="187" spans="1:4" hidden="1">
       <c r="A187" t="s">
         <v>132</v>
       </c>
@@ -3626,7 +3629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:4">
+    <row r="188" spans="1:4" hidden="1">
       <c r="A188" t="s">
         <v>132</v>
       </c>
@@ -3640,7 +3643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:4">
+    <row r="189" spans="1:4" hidden="1">
       <c r="A189" t="s">
         <v>132</v>
       </c>
@@ -3654,7 +3657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:4">
+    <row r="190" spans="1:4" hidden="1">
       <c r="A190" t="s">
         <v>132</v>
       </c>
@@ -3668,7 +3671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:4">
+    <row r="191" spans="1:4" hidden="1">
       <c r="A191" t="s">
         <v>132</v>
       </c>
@@ -3679,7 +3682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:4">
+    <row r="192" spans="1:4" hidden="1">
       <c r="A192" t="s">
         <v>132</v>
       </c>
@@ -3690,7 +3693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:4">
+    <row r="193" spans="1:4" hidden="1">
       <c r="A193" t="s">
         <v>132</v>
       </c>
@@ -3701,7 +3704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:4">
+    <row r="194" spans="1:4" hidden="1">
       <c r="A194" t="s">
         <v>132</v>
       </c>
@@ -3715,7 +3718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:4">
+    <row r="195" spans="1:4" hidden="1">
       <c r="A195" t="s">
         <v>132</v>
       </c>
@@ -3729,7 +3732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:4">
+    <row r="196" spans="1:4" hidden="1">
       <c r="A196" t="s">
         <v>132</v>
       </c>
@@ -3743,7 +3746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:4">
+    <row r="197" spans="1:4" hidden="1">
       <c r="A197" t="s">
         <v>132</v>
       </c>
@@ -3757,7 +3760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:4">
+    <row r="198" spans="1:4" hidden="1">
       <c r="A198" t="s">
         <v>132</v>
       </c>
@@ -3771,7 +3774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:4">
+    <row r="199" spans="1:4" hidden="1">
       <c r="A199" t="s">
         <v>132</v>
       </c>
@@ -3785,7 +3788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:4">
+    <row r="200" spans="1:4" hidden="1">
       <c r="A200" t="s">
         <v>132</v>
       </c>
@@ -3799,7 +3802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:4">
+    <row r="201" spans="1:4" hidden="1">
       <c r="A201" t="s">
         <v>132</v>
       </c>
@@ -3813,7 +3816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:4">
+    <row r="202" spans="1:4" hidden="1">
       <c r="A202" t="s">
         <v>132</v>
       </c>
@@ -3827,7 +3830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:4">
+    <row r="203" spans="1:4" hidden="1">
       <c r="A203" t="s">
         <v>132</v>
       </c>
@@ -3841,7 +3844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:4">
+    <row r="204" spans="1:4" hidden="1">
       <c r="A204" t="s">
         <v>132</v>
       </c>
@@ -3855,7 +3858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:4">
+    <row r="205" spans="1:4" hidden="1">
       <c r="A205" t="s">
         <v>132</v>
       </c>
@@ -3869,7 +3872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:4">
+    <row r="206" spans="1:4" hidden="1">
       <c r="A206" t="s">
         <v>132</v>
       </c>
@@ -3883,7 +3886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:4">
+    <row r="207" spans="1:4" hidden="1">
       <c r="A207" t="s">
         <v>132</v>
       </c>
@@ -3894,7 +3897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:4">
+    <row r="208" spans="1:4" hidden="1">
       <c r="A208" t="s">
         <v>132</v>
       </c>
@@ -3905,7 +3908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:4">
+    <row r="209" spans="1:4" hidden="1">
       <c r="A209" t="s">
         <v>132</v>
       </c>
@@ -3916,7 +3919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:4">
+    <row r="210" spans="1:4" hidden="1">
       <c r="A210" t="s">
         <v>132</v>
       </c>
@@ -3927,7 +3930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:4">
+    <row r="211" spans="1:4" hidden="1">
       <c r="A211" t="s">
         <v>132</v>
       </c>
@@ -7768,7 +7771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="525" spans="1:4" hidden="1">
+    <row r="525" spans="1:4">
       <c r="A525" t="s">
         <v>296</v>
       </c>
@@ -7782,7 +7785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="526" spans="1:4" hidden="1">
+    <row r="526" spans="1:4">
       <c r="A526" t="s">
         <v>296</v>
       </c>
@@ -7793,7 +7796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="527" spans="1:4" hidden="1">
+    <row r="527" spans="1:4">
       <c r="A527" t="s">
         <v>296</v>
       </c>
@@ -7804,7 +7807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="528" spans="1:4" hidden="1">
+    <row r="528" spans="1:4">
       <c r="A528" t="s">
         <v>296</v>
       </c>
@@ -7815,7 +7818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="529" spans="1:4" hidden="1">
+    <row r="529" spans="1:4">
       <c r="A529" t="s">
         <v>296</v>
       </c>
@@ -7826,7 +7829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="530" spans="1:4" hidden="1">
+    <row r="530" spans="1:4">
       <c r="A530" t="s">
         <v>296</v>
       </c>
@@ -7840,7 +7843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="531" spans="1:4" hidden="1">
+    <row r="531" spans="1:4">
       <c r="A531" t="s">
         <v>296</v>
       </c>
@@ -7854,7 +7857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="532" spans="1:4" hidden="1">
+    <row r="532" spans="1:4">
       <c r="A532" t="s">
         <v>296</v>
       </c>
@@ -7865,7 +7868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="533" spans="1:4" hidden="1">
+    <row r="533" spans="1:4">
       <c r="A533" t="s">
         <v>296</v>
       </c>
@@ -7879,7 +7882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="534" spans="1:4" hidden="1">
+    <row r="534" spans="1:4">
       <c r="A534" t="s">
         <v>296</v>
       </c>
@@ -7893,7 +7896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="535" spans="1:4" hidden="1">
+    <row r="535" spans="1:4">
       <c r="A535" t="s">
         <v>296</v>
       </c>
@@ -7907,7 +7910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="536" spans="1:4" hidden="1">
+    <row r="536" spans="1:4">
       <c r="A536" t="s">
         <v>296</v>
       </c>
@@ -7921,7 +7924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="537" spans="1:4" hidden="1">
+    <row r="537" spans="1:4">
       <c r="A537" t="s">
         <v>296</v>
       </c>
@@ -7935,7 +7938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="538" spans="1:4" hidden="1">
+    <row r="538" spans="1:4">
       <c r="A538" t="s">
         <v>296</v>
       </c>
@@ -7949,7 +7952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="539" spans="1:4" hidden="1">
+    <row r="539" spans="1:4">
       <c r="A539" t="s">
         <v>296</v>
       </c>
@@ -7960,7 +7963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="540" spans="1:4" hidden="1">
+    <row r="540" spans="1:4">
       <c r="A540" t="s">
         <v>296</v>
       </c>
@@ -7971,7 +7974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="541" spans="1:4" hidden="1">
+    <row r="541" spans="1:4">
       <c r="A541" t="s">
         <v>296</v>
       </c>
@@ -7982,7 +7985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="542" spans="1:4" hidden="1">
+    <row r="542" spans="1:4">
       <c r="A542" t="s">
         <v>296</v>
       </c>
@@ -7993,7 +7996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="543" spans="1:4" hidden="1">
+    <row r="543" spans="1:4">
       <c r="A543" t="s">
         <v>296</v>
       </c>
@@ -8004,7 +8007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="544" spans="1:4" hidden="1">
+    <row r="544" spans="1:4">
       <c r="A544" t="s">
         <v>296</v>
       </c>
@@ -8015,7 +8018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="545" spans="1:4" hidden="1">
+    <row r="545" spans="1:4">
       <c r="A545" t="s">
         <v>296</v>
       </c>
@@ -8026,7 +8029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="546" spans="1:4" hidden="1">
+    <row r="546" spans="1:4">
       <c r="A546" t="s">
         <v>296</v>
       </c>
@@ -8040,7 +8043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="547" spans="1:4" hidden="1">
+    <row r="547" spans="1:4">
       <c r="A547" t="s">
         <v>296</v>
       </c>
@@ -8054,7 +8057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="548" spans="1:4" hidden="1">
+    <row r="548" spans="1:4">
       <c r="A548" t="s">
         <v>296</v>
       </c>
@@ -8068,7 +8071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="549" spans="1:4" hidden="1">
+    <row r="549" spans="1:4">
       <c r="A549" t="s">
         <v>296</v>
       </c>
@@ -8082,7 +8085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="550" spans="1:4" hidden="1">
+    <row r="550" spans="1:4">
       <c r="A550" t="s">
         <v>296</v>
       </c>
@@ -8093,7 +8096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="551" spans="1:4" hidden="1">
+    <row r="551" spans="1:4">
       <c r="A551" t="s">
         <v>296</v>
       </c>
@@ -8104,7 +8107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="552" spans="1:4" hidden="1">
+    <row r="552" spans="1:4">
       <c r="A552" t="s">
         <v>296</v>
       </c>
@@ -8115,7 +8118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="553" spans="1:4" hidden="1">
+    <row r="553" spans="1:4">
       <c r="A553" t="s">
         <v>296</v>
       </c>
@@ -8126,7 +8129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="554" spans="1:4" hidden="1">
+    <row r="554" spans="1:4">
       <c r="A554" t="s">
         <v>296</v>
       </c>
@@ -8137,7 +8140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="555" spans="1:4" hidden="1">
+    <row r="555" spans="1:4">
       <c r="A555" t="s">
         <v>296</v>
       </c>
@@ -8148,7 +8151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="556" spans="1:4" hidden="1">
+    <row r="556" spans="1:4">
       <c r="A556" t="s">
         <v>296</v>
       </c>
@@ -8159,7 +8162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="557" spans="1:4" hidden="1">
+    <row r="557" spans="1:4">
       <c r="A557" t="s">
         <v>296</v>
       </c>
@@ -8170,7 +8173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="558" spans="1:4" hidden="1">
+    <row r="558" spans="1:4">
       <c r="A558" t="s">
         <v>296</v>
       </c>
@@ -8184,26 +8187,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="559" spans="1:4" hidden="1">
+    <row r="559" spans="1:4">
       <c r="A559" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
       <c r="B559" t="s">
-        <v>5</v>
+        <v>335</v>
       </c>
       <c r="C559">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="560" spans="1:4" hidden="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="560" spans="1:4">
       <c r="A560" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
       <c r="B560" t="s">
-        <v>71</v>
+        <v>337</v>
       </c>
       <c r="C560">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="561" spans="1:4" hidden="1">
@@ -8211,10 +8214,10 @@
         <v>309</v>
       </c>
       <c r="B561" t="s">
-        <v>69</v>
+        <v>5</v>
       </c>
       <c r="C561">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="562" spans="1:4" hidden="1">
@@ -8222,7 +8225,7 @@
         <v>309</v>
       </c>
       <c r="B562" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C562">
         <v>1</v>
@@ -8233,10 +8236,10 @@
         <v>309</v>
       </c>
       <c r="B563" t="s">
-        <v>310</v>
+        <v>69</v>
       </c>
       <c r="C563">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="564" spans="1:4" hidden="1">
@@ -8244,7 +8247,7 @@
         <v>309</v>
       </c>
       <c r="B564" t="s">
-        <v>311</v>
+        <v>70</v>
       </c>
       <c r="C564">
         <v>1</v>
@@ -8255,10 +8258,10 @@
         <v>309</v>
       </c>
       <c r="B565" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C565">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="566" spans="1:4" hidden="1">
@@ -8266,10 +8269,10 @@
         <v>309</v>
       </c>
       <c r="B566" t="s">
-        <v>50</v>
+        <v>311</v>
       </c>
       <c r="C566">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="567" spans="1:4" hidden="1">
@@ -8277,7 +8280,7 @@
         <v>309</v>
       </c>
       <c r="B567" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C567">
         <v>0</v>
@@ -8288,13 +8291,10 @@
         <v>309</v>
       </c>
       <c r="B568" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C568">
         <v>0</v>
-      </c>
-      <c r="D568">
-        <v>1</v>
       </c>
     </row>
     <row r="569" spans="1:4" hidden="1">
@@ -8302,13 +8302,10 @@
         <v>309</v>
       </c>
       <c r="B569" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C569">
         <v>0</v>
-      </c>
-      <c r="D569">
-        <v>1</v>
       </c>
     </row>
     <row r="570" spans="1:4" hidden="1">
@@ -8316,10 +8313,13 @@
         <v>309</v>
       </c>
       <c r="B570" t="s">
-        <v>315</v>
+        <v>55</v>
       </c>
       <c r="C570">
         <v>0</v>
+      </c>
+      <c r="D570">
+        <v>1</v>
       </c>
     </row>
     <row r="571" spans="1:4" hidden="1">
@@ -8327,7 +8327,7 @@
         <v>309</v>
       </c>
       <c r="B571" t="s">
-        <v>221</v>
+        <v>314</v>
       </c>
       <c r="C571">
         <v>0</v>
@@ -8341,7 +8341,7 @@
         <v>309</v>
       </c>
       <c r="B572" t="s">
-        <v>112</v>
+        <v>315</v>
       </c>
       <c r="C572">
         <v>0</v>
@@ -8352,7 +8352,7 @@
         <v>309</v>
       </c>
       <c r="B573" t="s">
-        <v>316</v>
+        <v>221</v>
       </c>
       <c r="C573">
         <v>0</v>
@@ -8366,13 +8366,10 @@
         <v>309</v>
       </c>
       <c r="B574" t="s">
-        <v>18</v>
+        <v>112</v>
       </c>
       <c r="C574">
         <v>0</v>
-      </c>
-      <c r="D574">
-        <v>1</v>
       </c>
     </row>
     <row r="575" spans="1:4" hidden="1">
@@ -8380,7 +8377,7 @@
         <v>309</v>
       </c>
       <c r="B575" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C575">
         <v>0</v>
@@ -8394,7 +8391,7 @@
         <v>309</v>
       </c>
       <c r="B576" t="s">
-        <v>318</v>
+        <v>18</v>
       </c>
       <c r="C576">
         <v>0</v>
@@ -8408,10 +8405,13 @@
         <v>309</v>
       </c>
       <c r="B577" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C577">
         <v>0</v>
+      </c>
+      <c r="D577">
+        <v>1</v>
       </c>
     </row>
     <row r="578" spans="1:4" hidden="1">
@@ -8419,7 +8419,7 @@
         <v>309</v>
       </c>
       <c r="B578" t="s">
-        <v>304</v>
+        <v>318</v>
       </c>
       <c r="C578">
         <v>0</v>
@@ -8433,7 +8433,7 @@
         <v>309</v>
       </c>
       <c r="B579" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C579">
         <v>0</v>
@@ -8444,10 +8444,13 @@
         <v>309</v>
       </c>
       <c r="B580" t="s">
-        <v>321</v>
+        <v>304</v>
       </c>
       <c r="C580">
         <v>0</v>
+      </c>
+      <c r="D580">
+        <v>1</v>
       </c>
     </row>
     <row r="581" spans="1:4" hidden="1">
@@ -8455,7 +8458,7 @@
         <v>309</v>
       </c>
       <c r="B581" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C581">
         <v>0</v>
@@ -8466,7 +8469,7 @@
         <v>309</v>
       </c>
       <c r="B582" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C582">
         <v>0</v>
@@ -8477,7 +8480,7 @@
         <v>309</v>
       </c>
       <c r="B583" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C583">
         <v>0</v>
@@ -8488,7 +8491,7 @@
         <v>309</v>
       </c>
       <c r="B584" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C584">
         <v>0</v>
@@ -8499,7 +8502,7 @@
         <v>309</v>
       </c>
       <c r="B585" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C585">
         <v>0</v>
@@ -8510,7 +8513,7 @@
         <v>309</v>
       </c>
       <c r="B586" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C586">
         <v>0</v>
@@ -8521,7 +8524,7 @@
         <v>309</v>
       </c>
       <c r="B587" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C587">
         <v>0</v>
@@ -8532,7 +8535,7 @@
         <v>309</v>
       </c>
       <c r="B588" t="s">
-        <v>51</v>
+        <v>327</v>
       </c>
       <c r="C588">
         <v>0</v>
@@ -8543,7 +8546,7 @@
         <v>309</v>
       </c>
       <c r="B589" t="s">
-        <v>52</v>
+        <v>328</v>
       </c>
       <c r="C589">
         <v>0</v>
@@ -8554,7 +8557,7 @@
         <v>309</v>
       </c>
       <c r="B590" t="s">
-        <v>329</v>
+        <v>51</v>
       </c>
       <c r="C590">
         <v>0</v>
@@ -8565,7 +8568,7 @@
         <v>309</v>
       </c>
       <c r="B591" t="s">
-        <v>330</v>
+        <v>52</v>
       </c>
       <c r="C591">
         <v>0</v>
@@ -8576,7 +8579,7 @@
         <v>309</v>
       </c>
       <c r="B592" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C592">
         <v>0</v>
@@ -8587,12 +8590,34 @@
         <v>309</v>
       </c>
       <c r="B593" t="s">
+        <v>330</v>
+      </c>
+      <c r="C593">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="594" spans="1:4" hidden="1">
+      <c r="A594" t="s">
+        <v>309</v>
+      </c>
+      <c r="B594" t="s">
+        <v>331</v>
+      </c>
+      <c r="C594">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="595" spans="1:4" hidden="1">
+      <c r="A595" t="s">
+        <v>309</v>
+      </c>
+      <c r="B595" t="s">
         <v>332</v>
       </c>
-      <c r="C593">
-        <v>0</v>
-      </c>
-      <c r="D593">
+      <c r="C595">
+        <v>0</v>
+      </c>
+      <c r="D595">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização documentação LN e ODS
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Mapeamento ODS_LN.xlsx
+++ b/Documentação/Planilhas/Mapeamento ODS_LN.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="135" windowWidth="20490" windowHeight="7950"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="349">
   <si>
     <t>TABELA</t>
   </si>
@@ -807,9 +807,6 @@
     <t>CD_CEP_FATURA</t>
   </si>
   <si>
-    <t>COD_CLIENTE_ENTREGA</t>
-  </si>
-  <si>
     <t>CD_PAIS_ENTREGA</t>
   </si>
   <si>
@@ -825,12 +822,6 @@
     <t>NR_CAMPANHA_B2B</t>
   </si>
   <si>
-    <t>PRAZO_TRANSIT_TIME</t>
-  </si>
-  <si>
-    <t>PRAZO_CD</t>
-  </si>
-  <si>
     <t>NR_PEDIDO_GARANTIA</t>
   </si>
   <si>
@@ -1066,6 +1057,12 @@
   </si>
   <si>
     <t>DT_REVERSAO</t>
+  </si>
+  <si>
+    <t>QT_PRAZO_TRANSIT_TIME</t>
+  </si>
+  <si>
+    <t>QT_PRAZO_CD</t>
   </si>
 </sst>
 </file>
@@ -1426,8 +1423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D610"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A86" sqref="A86:C86"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A475" workbookViewId="0">
+      <selection activeCell="B495" sqref="B495"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1445,10 +1442,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1884,7 +1881,7 @@
         <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -1939,7 +1936,7 @@
         <v>37</v>
       </c>
       <c r="B41" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -2349,7 +2346,7 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B75" t="s">
         <v>36</v>
@@ -2360,7 +2357,7 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B76" t="s">
         <v>5</v>
@@ -2371,7 +2368,7 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B77" t="s">
         <v>6</v>
@@ -2382,10 +2379,10 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B78" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C78">
         <v>0</v>
@@ -2393,10 +2390,10 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B79" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C79">
         <v>0</v>
@@ -2404,10 +2401,10 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
+        <v>337</v>
+      </c>
+      <c r="B80" t="s">
         <v>340</v>
-      </c>
-      <c r="B80" t="s">
-        <v>343</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -2415,10 +2412,10 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B81" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -2426,10 +2423,10 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B82" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C82">
         <v>0</v>
@@ -2437,10 +2434,10 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B83" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C83">
         <v>0</v>
@@ -2448,10 +2445,10 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B84" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -2459,10 +2456,10 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B85" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C85">
         <v>0</v>
@@ -2470,10 +2467,10 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B86" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -3346,7 +3343,7 @@
         <v>60</v>
       </c>
       <c r="B164" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C164">
         <v>0</v>
@@ -3357,7 +3354,7 @@
         <v>60</v>
       </c>
       <c r="B165" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C165">
         <v>0</v>
@@ -3368,7 +3365,7 @@
         <v>60</v>
       </c>
       <c r="B166" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C166">
         <v>0</v>
@@ -4106,7 +4103,7 @@
         <v>132</v>
       </c>
       <c r="B223" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C223">
         <v>0</v>
@@ -7343,7 +7340,7 @@
         <v>249</v>
       </c>
       <c r="B484" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C484">
         <v>0</v>
@@ -7365,7 +7362,7 @@
         <v>249</v>
       </c>
       <c r="B486" t="s">
-        <v>263</v>
+        <v>67</v>
       </c>
       <c r="C486">
         <v>0</v>
@@ -7387,7 +7384,7 @@
         <v>249</v>
       </c>
       <c r="B488" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C488">
         <v>0</v>
@@ -7398,7 +7395,7 @@
         <v>249</v>
       </c>
       <c r="B489" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C489">
         <v>0</v>
@@ -7409,7 +7406,7 @@
         <v>249</v>
       </c>
       <c r="B490" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C490">
         <v>0</v>
@@ -7431,7 +7428,7 @@
         <v>249</v>
       </c>
       <c r="B492" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C492">
         <v>0</v>
@@ -7442,7 +7439,7 @@
         <v>249</v>
       </c>
       <c r="B493" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C493">
         <v>0</v>
@@ -7453,7 +7450,7 @@
         <v>249</v>
       </c>
       <c r="B494" t="s">
-        <v>269</v>
+        <v>347</v>
       </c>
       <c r="C494">
         <v>0</v>
@@ -7467,7 +7464,7 @@
         <v>249</v>
       </c>
       <c r="B495" t="s">
-        <v>270</v>
+        <v>348</v>
       </c>
       <c r="C495">
         <v>0</v>
@@ -7503,7 +7500,7 @@
         <v>249</v>
       </c>
       <c r="B498" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C498">
         <v>0</v>
@@ -7514,7 +7511,7 @@
         <v>249</v>
       </c>
       <c r="B499" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C499">
         <v>0</v>
@@ -7528,7 +7525,7 @@
         <v>249</v>
       </c>
       <c r="B500" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C500">
         <v>0</v>
@@ -7539,7 +7536,7 @@
         <v>249</v>
       </c>
       <c r="B501" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C501">
         <v>0</v>
@@ -7550,7 +7547,7 @@
         <v>249</v>
       </c>
       <c r="B502" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C502">
         <v>0</v>
@@ -7594,7 +7591,7 @@
         <v>249</v>
       </c>
       <c r="B506" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C506">
         <v>0</v>
@@ -7605,7 +7602,7 @@
         <v>249</v>
       </c>
       <c r="B507" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C507">
         <v>0</v>
@@ -7619,7 +7616,7 @@
         <v>249</v>
       </c>
       <c r="B508" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C508">
         <v>0</v>
@@ -7644,7 +7641,7 @@
         <v>249</v>
       </c>
       <c r="B510" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C510">
         <v>0</v>
@@ -7652,7 +7649,7 @@
     </row>
     <row r="511" spans="1:4">
       <c r="A511" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B511" t="s">
         <v>5</v>
@@ -7663,7 +7660,7 @@
     </row>
     <row r="512" spans="1:4">
       <c r="A512" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B512" t="s">
         <v>69</v>
@@ -7674,7 +7671,7 @@
     </row>
     <row r="513" spans="1:3">
       <c r="A513" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B513" t="s">
         <v>70</v>
@@ -7685,7 +7682,7 @@
     </row>
     <row r="514" spans="1:3">
       <c r="A514" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B514" t="s">
         <v>71</v>
@@ -7696,7 +7693,7 @@
     </row>
     <row r="515" spans="1:3">
       <c r="A515" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B515" t="s">
         <v>66</v>
@@ -7707,10 +7704,10 @@
     </row>
     <row r="516" spans="1:3">
       <c r="A516" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B516" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C516">
         <v>0</v>
@@ -7718,7 +7715,7 @@
     </row>
     <row r="517" spans="1:3">
       <c r="A517" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B517" t="s">
         <v>109</v>
@@ -7729,7 +7726,7 @@
     </row>
     <row r="518" spans="1:3">
       <c r="A518" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B518" t="s">
         <v>261</v>
@@ -7740,10 +7737,10 @@
     </row>
     <row r="519" spans="1:3">
       <c r="A519" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B519" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C519">
         <v>0</v>
@@ -7751,7 +7748,7 @@
     </row>
     <row r="520" spans="1:3">
       <c r="A520" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B520" t="s">
         <v>262</v>
@@ -7762,10 +7759,10 @@
     </row>
     <row r="521" spans="1:3">
       <c r="A521" t="s">
+        <v>276</v>
+      </c>
+      <c r="B521" t="s">
         <v>279</v>
-      </c>
-      <c r="B521" t="s">
-        <v>282</v>
       </c>
       <c r="C521">
         <v>0</v>
@@ -7773,10 +7770,10 @@
     </row>
     <row r="522" spans="1:3">
       <c r="A522" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B522" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C522">
         <v>0</v>
@@ -7784,10 +7781,10 @@
     </row>
     <row r="523" spans="1:3">
       <c r="A523" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B523" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C523">
         <v>0</v>
@@ -7795,10 +7792,10 @@
     </row>
     <row r="524" spans="1:3">
       <c r="A524" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B524" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C524">
         <v>0</v>
@@ -7806,10 +7803,10 @@
     </row>
     <row r="525" spans="1:3">
       <c r="A525" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B525" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C525">
         <v>0</v>
@@ -7817,7 +7814,7 @@
     </row>
     <row r="526" spans="1:3">
       <c r="A526" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B526" t="s">
         <v>67</v>
@@ -7828,7 +7825,7 @@
     </row>
     <row r="527" spans="1:3">
       <c r="A527" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B527" t="s">
         <v>110</v>
@@ -7839,10 +7836,10 @@
     </row>
     <row r="528" spans="1:3">
       <c r="A528" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B528" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C528">
         <v>0</v>
@@ -7850,10 +7847,10 @@
     </row>
     <row r="529" spans="1:4">
       <c r="A529" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B529" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C529">
         <v>0</v>
@@ -7861,10 +7858,10 @@
     </row>
     <row r="530" spans="1:4">
       <c r="A530" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B530" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C530">
         <v>0</v>
@@ -7872,10 +7869,10 @@
     </row>
     <row r="531" spans="1:4">
       <c r="A531" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B531" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C531">
         <v>0</v>
@@ -7883,10 +7880,10 @@
     </row>
     <row r="532" spans="1:4">
       <c r="A532" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B532" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C532">
         <v>0</v>
@@ -7894,10 +7891,10 @@
     </row>
     <row r="533" spans="1:4">
       <c r="A533" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B533" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C533">
         <v>0</v>
@@ -7905,10 +7902,10 @@
     </row>
     <row r="534" spans="1:4">
       <c r="A534" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B534" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C534">
         <v>0</v>
@@ -7916,10 +7913,10 @@
     </row>
     <row r="535" spans="1:4">
       <c r="A535" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B535" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C535">
         <v>0</v>
@@ -7927,10 +7924,10 @@
     </row>
     <row r="536" spans="1:4">
       <c r="A536" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B536" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C536">
         <v>0</v>
@@ -7938,10 +7935,10 @@
     </row>
     <row r="537" spans="1:4">
       <c r="A537" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B537" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C537">
         <v>0</v>
@@ -7952,10 +7949,10 @@
     </row>
     <row r="538" spans="1:4">
       <c r="A538" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B538" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C538">
         <v>0</v>
@@ -7966,7 +7963,7 @@
     </row>
     <row r="539" spans="1:4">
       <c r="A539" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B539" t="s">
         <v>126</v>
@@ -7977,7 +7974,7 @@
     </row>
     <row r="540" spans="1:4">
       <c r="A540" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B540" t="s">
         <v>33</v>
@@ -7991,7 +7988,7 @@
     </row>
     <row r="541" spans="1:4">
       <c r="A541" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B541" t="s">
         <v>5</v>
@@ -8002,7 +7999,7 @@
     </row>
     <row r="542" spans="1:4">
       <c r="A542" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B542" t="s">
         <v>112</v>
@@ -8013,7 +8010,7 @@
     </row>
     <row r="543" spans="1:4">
       <c r="A543" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B543" t="s">
         <v>71</v>
@@ -8024,7 +8021,7 @@
     </row>
     <row r="544" spans="1:4">
       <c r="A544" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B544" t="s">
         <v>251</v>
@@ -8035,7 +8032,7 @@
     </row>
     <row r="545" spans="1:4">
       <c r="A545" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B545" t="s">
         <v>120</v>
@@ -8049,7 +8046,7 @@
     </row>
     <row r="546" spans="1:4">
       <c r="A546" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B546" t="s">
         <v>225</v>
@@ -8063,7 +8060,7 @@
     </row>
     <row r="547" spans="1:4">
       <c r="A547" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B547" t="s">
         <v>256</v>
@@ -8074,7 +8071,7 @@
     </row>
     <row r="548" spans="1:4">
       <c r="A548" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B548" t="s">
         <v>80</v>
@@ -8088,10 +8085,10 @@
     </row>
     <row r="549" spans="1:4">
       <c r="A549" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B549" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C549">
         <v>0</v>
@@ -8102,10 +8099,10 @@
     </row>
     <row r="550" spans="1:4">
       <c r="A550" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B550" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C550">
         <v>0</v>
@@ -8116,7 +8113,7 @@
     </row>
     <row r="551" spans="1:4">
       <c r="A551" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B551" t="s">
         <v>106</v>
@@ -8130,7 +8127,7 @@
     </row>
     <row r="552" spans="1:4">
       <c r="A552" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B552" t="s">
         <v>255</v>
@@ -8144,7 +8141,7 @@
     </row>
     <row r="553" spans="1:4">
       <c r="A553" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B553" t="s">
         <v>86</v>
@@ -8158,7 +8155,7 @@
     </row>
     <row r="554" spans="1:4">
       <c r="A554" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B554" t="s">
         <v>116</v>
@@ -8169,7 +8166,7 @@
     </row>
     <row r="555" spans="1:4">
       <c r="A555" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B555" t="s">
         <v>126</v>
@@ -8180,10 +8177,10 @@
     </row>
     <row r="556" spans="1:4">
       <c r="A556" t="s">
+        <v>292</v>
+      </c>
+      <c r="B556" t="s">
         <v>295</v>
-      </c>
-      <c r="B556" t="s">
-        <v>298</v>
       </c>
       <c r="C556">
         <v>0</v>
@@ -8191,7 +8188,7 @@
     </row>
     <row r="557" spans="1:4">
       <c r="A557" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B557" t="s">
         <v>54</v>
@@ -8202,10 +8199,10 @@
     </row>
     <row r="558" spans="1:4">
       <c r="A558" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B558" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C558">
         <v>0</v>
@@ -8213,10 +8210,10 @@
     </row>
     <row r="559" spans="1:4">
       <c r="A559" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B559" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C559">
         <v>0</v>
@@ -8224,10 +8221,10 @@
     </row>
     <row r="560" spans="1:4">
       <c r="A560" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B560" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C560">
         <v>0</v>
@@ -8235,10 +8232,10 @@
     </row>
     <row r="561" spans="1:4">
       <c r="A561" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B561" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C561">
         <v>0</v>
@@ -8249,10 +8246,10 @@
     </row>
     <row r="562" spans="1:4">
       <c r="A562" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B562" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C562">
         <v>0</v>
@@ -8263,7 +8260,7 @@
     </row>
     <row r="563" spans="1:4">
       <c r="A563" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B563" t="s">
         <v>89</v>
@@ -8277,10 +8274,10 @@
     </row>
     <row r="564" spans="1:4">
       <c r="A564" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B564" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C564">
         <v>0</v>
@@ -8291,7 +8288,7 @@
     </row>
     <row r="565" spans="1:4">
       <c r="A565" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B565" t="s">
         <v>6</v>
@@ -8302,7 +8299,7 @@
     </row>
     <row r="566" spans="1:4">
       <c r="A566" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B566" t="s">
         <v>34</v>
@@ -8313,10 +8310,10 @@
     </row>
     <row r="567" spans="1:4">
       <c r="A567" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B567" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C567">
         <v>0</v>
@@ -8324,7 +8321,7 @@
     </row>
     <row r="568" spans="1:4">
       <c r="A568" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B568" t="s">
         <v>69</v>
@@ -8335,7 +8332,7 @@
     </row>
     <row r="569" spans="1:4">
       <c r="A569" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B569" t="s">
         <v>70</v>
@@ -8346,10 +8343,10 @@
     </row>
     <row r="570" spans="1:4">
       <c r="A570" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B570" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C570">
         <v>0</v>
@@ -8357,10 +8354,10 @@
     </row>
     <row r="571" spans="1:4">
       <c r="A571" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B571" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C571">
         <v>0</v>
@@ -8368,7 +8365,7 @@
     </row>
     <row r="572" spans="1:4">
       <c r="A572" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B572" t="s">
         <v>257</v>
@@ -8379,7 +8376,7 @@
     </row>
     <row r="573" spans="1:4">
       <c r="A573" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B573" t="s">
         <v>78</v>
@@ -8393,10 +8390,10 @@
     </row>
     <row r="574" spans="1:4">
       <c r="A574" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B574" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C574">
         <v>0</v>
@@ -8404,10 +8401,10 @@
     </row>
     <row r="575" spans="1:4">
       <c r="A575" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B575" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C575">
         <v>0</v>
@@ -8415,10 +8412,10 @@
     </row>
     <row r="576" spans="1:4">
       <c r="A576" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B576" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C576">
         <v>0</v>
@@ -8429,7 +8426,7 @@
     </row>
     <row r="577" spans="1:4">
       <c r="A577" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B577" t="s">
         <v>5</v>
@@ -8440,7 +8437,7 @@
     </row>
     <row r="578" spans="1:4">
       <c r="A578" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B578" t="s">
         <v>71</v>
@@ -8451,7 +8448,7 @@
     </row>
     <row r="579" spans="1:4">
       <c r="A579" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B579" t="s">
         <v>69</v>
@@ -8462,7 +8459,7 @@
     </row>
     <row r="580" spans="1:4">
       <c r="A580" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B580" t="s">
         <v>70</v>
@@ -8473,10 +8470,10 @@
     </row>
     <row r="581" spans="1:4">
       <c r="A581" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B581" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C581">
         <v>1</v>
@@ -8484,10 +8481,10 @@
     </row>
     <row r="582" spans="1:4">
       <c r="A582" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B582" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C582">
         <v>1</v>
@@ -8495,10 +8492,10 @@
     </row>
     <row r="583" spans="1:4">
       <c r="A583" t="s">
+        <v>305</v>
+      </c>
+      <c r="B583" t="s">
         <v>308</v>
-      </c>
-      <c r="B583" t="s">
-        <v>311</v>
       </c>
       <c r="C583">
         <v>0</v>
@@ -8506,7 +8503,7 @@
     </row>
     <row r="584" spans="1:4">
       <c r="A584" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B584" t="s">
         <v>50</v>
@@ -8517,10 +8514,10 @@
     </row>
     <row r="585" spans="1:4">
       <c r="A585" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B585" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C585">
         <v>0</v>
@@ -8528,7 +8525,7 @@
     </row>
     <row r="586" spans="1:4">
       <c r="A586" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B586" t="s">
         <v>55</v>
@@ -8542,10 +8539,10 @@
     </row>
     <row r="587" spans="1:4">
       <c r="A587" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B587" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C587">
         <v>0</v>
@@ -8556,10 +8553,10 @@
     </row>
     <row r="588" spans="1:4">
       <c r="A588" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B588" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C588">
         <v>0</v>
@@ -8567,7 +8564,7 @@
     </row>
     <row r="589" spans="1:4">
       <c r="A589" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B589" t="s">
         <v>221</v>
@@ -8581,7 +8578,7 @@
     </row>
     <row r="590" spans="1:4">
       <c r="A590" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B590" t="s">
         <v>112</v>
@@ -8592,10 +8589,10 @@
     </row>
     <row r="591" spans="1:4">
       <c r="A591" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B591" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C591">
         <v>0</v>
@@ -8606,7 +8603,7 @@
     </row>
     <row r="592" spans="1:4">
       <c r="A592" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B592" t="s">
         <v>18</v>
@@ -8620,10 +8617,10 @@
     </row>
     <row r="593" spans="1:4">
       <c r="A593" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B593" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C593">
         <v>0</v>
@@ -8634,10 +8631,10 @@
     </row>
     <row r="594" spans="1:4">
       <c r="A594" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B594" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C594">
         <v>0</v>
@@ -8648,10 +8645,10 @@
     </row>
     <row r="595" spans="1:4">
       <c r="A595" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B595" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C595">
         <v>0</v>
@@ -8659,10 +8656,10 @@
     </row>
     <row r="596" spans="1:4">
       <c r="A596" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B596" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C596">
         <v>0</v>
@@ -8673,10 +8670,10 @@
     </row>
     <row r="597" spans="1:4">
       <c r="A597" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B597" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C597">
         <v>0</v>
@@ -8684,10 +8681,10 @@
     </row>
     <row r="598" spans="1:4">
       <c r="A598" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B598" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C598">
         <v>0</v>
@@ -8695,10 +8692,10 @@
     </row>
     <row r="599" spans="1:4">
       <c r="A599" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B599" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C599">
         <v>0</v>
@@ -8706,10 +8703,10 @@
     </row>
     <row r="600" spans="1:4">
       <c r="A600" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B600" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C600">
         <v>0</v>
@@ -8717,10 +8714,10 @@
     </row>
     <row r="601" spans="1:4">
       <c r="A601" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B601" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C601">
         <v>0</v>
@@ -8728,10 +8725,10 @@
     </row>
     <row r="602" spans="1:4">
       <c r="A602" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B602" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C602">
         <v>0</v>
@@ -8739,10 +8736,10 @@
     </row>
     <row r="603" spans="1:4">
       <c r="A603" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B603" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C603">
         <v>0</v>
@@ -8750,10 +8747,10 @@
     </row>
     <row r="604" spans="1:4">
       <c r="A604" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B604" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C604">
         <v>0</v>
@@ -8761,10 +8758,10 @@
     </row>
     <row r="605" spans="1:4">
       <c r="A605" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B605" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C605">
         <v>0</v>
@@ -8772,7 +8769,7 @@
     </row>
     <row r="606" spans="1:4">
       <c r="A606" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B606" t="s">
         <v>51</v>
@@ -8783,7 +8780,7 @@
     </row>
     <row r="607" spans="1:4">
       <c r="A607" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B607" t="s">
         <v>52</v>
@@ -8794,10 +8791,10 @@
     </row>
     <row r="608" spans="1:4">
       <c r="A608" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B608" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C608">
         <v>0</v>
@@ -8805,10 +8802,10 @@
     </row>
     <row r="609" spans="1:4">
       <c r="A609" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B609" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C609">
         <v>0</v>
@@ -8816,10 +8813,10 @@
     </row>
     <row r="610" spans="1:4">
       <c r="A610" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B610" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C610" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
Atualização Doc Mapeamento LN e ODS
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Mapeamento ODS_LN.xlsx
+++ b/Documentação/Planilhas/Mapeamento ODS_LN.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1402" uniqueCount="372">
   <si>
     <t>TABELA</t>
   </si>
@@ -1196,8 +1196,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:D699" totalsRowShown="0">
-  <autoFilter ref="A1:D699">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:D700" totalsRowShown="0">
+  <autoFilter ref="A1:D700">
     <filterColumn colId="0"/>
     <filterColumn colId="3"/>
   </autoFilter>
@@ -1496,10 +1496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D699"/>
+  <dimension ref="A1:D700"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A602" workbookViewId="0">
-      <selection activeCell="C692" sqref="C692"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A326" workbookViewId="0">
+      <selection activeCell="D343" sqref="D343"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5699,13 +5699,13 @@
     </row>
     <row r="343" spans="1:4">
       <c r="A343" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B343" t="s">
-        <v>5</v>
+        <v>235</v>
       </c>
       <c r="C343">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="344" spans="1:4">
@@ -5713,10 +5713,10 @@
         <v>205</v>
       </c>
       <c r="B344" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C344">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="345" spans="1:4">
@@ -5724,13 +5724,10 @@
         <v>205</v>
       </c>
       <c r="B345" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="C345">
         <v>0</v>
-      </c>
-      <c r="D345">
-        <v>1</v>
       </c>
     </row>
     <row r="346" spans="1:4">
@@ -5738,7 +5735,7 @@
         <v>205</v>
       </c>
       <c r="B346" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C346">
         <v>0</v>
@@ -5752,9 +5749,12 @@
         <v>205</v>
       </c>
       <c r="B347" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="C347">
+        <v>0</v>
+      </c>
+      <c r="D347">
         <v>1</v>
       </c>
     </row>
@@ -5763,10 +5763,10 @@
         <v>205</v>
       </c>
       <c r="B348" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C348">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="349" spans="1:4">
@@ -5774,7 +5774,7 @@
         <v>205</v>
       </c>
       <c r="B349" t="s">
-        <v>206</v>
+        <v>81</v>
       </c>
       <c r="C349">
         <v>0</v>
@@ -5785,7 +5785,7 @@
         <v>205</v>
       </c>
       <c r="B350" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C350">
         <v>0</v>
@@ -5796,7 +5796,7 @@
         <v>205</v>
       </c>
       <c r="B351" t="s">
-        <v>82</v>
+        <v>207</v>
       </c>
       <c r="C351">
         <v>0</v>
@@ -5807,7 +5807,7 @@
         <v>205</v>
       </c>
       <c r="B352" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C352">
         <v>0</v>
@@ -5818,7 +5818,7 @@
         <v>205</v>
       </c>
       <c r="B353" t="s">
-        <v>144</v>
+        <v>83</v>
       </c>
       <c r="C353">
         <v>0</v>
@@ -5829,7 +5829,7 @@
         <v>205</v>
       </c>
       <c r="B354" t="s">
-        <v>84</v>
+        <v>144</v>
       </c>
       <c r="C354">
         <v>0</v>
@@ -5840,7 +5840,7 @@
         <v>205</v>
       </c>
       <c r="B355" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C355">
         <v>0</v>
@@ -5851,7 +5851,7 @@
         <v>205</v>
       </c>
       <c r="B356" t="s">
-        <v>202</v>
+        <v>85</v>
       </c>
       <c r="C356">
         <v>0</v>
@@ -5862,7 +5862,7 @@
         <v>205</v>
       </c>
       <c r="B357" t="s">
-        <v>87</v>
+        <v>202</v>
       </c>
       <c r="C357">
         <v>0</v>
@@ -5873,7 +5873,7 @@
         <v>205</v>
       </c>
       <c r="B358" t="s">
-        <v>157</v>
+        <v>87</v>
       </c>
       <c r="C358">
         <v>0</v>
@@ -5884,7 +5884,7 @@
         <v>205</v>
       </c>
       <c r="B359" t="s">
-        <v>88</v>
+        <v>157</v>
       </c>
       <c r="C359">
         <v>0</v>
@@ -5895,7 +5895,7 @@
         <v>205</v>
       </c>
       <c r="B360" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C360">
         <v>0</v>
@@ -5906,13 +5906,10 @@
         <v>205</v>
       </c>
       <c r="B361" t="s">
-        <v>208</v>
+        <v>89</v>
       </c>
       <c r="C361">
         <v>0</v>
-      </c>
-      <c r="D361">
-        <v>1</v>
       </c>
     </row>
     <row r="362" spans="1:4">
@@ -5920,10 +5917,13 @@
         <v>205</v>
       </c>
       <c r="B362" t="s">
-        <v>90</v>
+        <v>208</v>
       </c>
       <c r="C362">
         <v>0</v>
+      </c>
+      <c r="D362">
+        <v>1</v>
       </c>
     </row>
     <row r="363" spans="1:4">
@@ -5931,7 +5931,7 @@
         <v>205</v>
       </c>
       <c r="B363" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C363">
         <v>0</v>
@@ -5942,7 +5942,7 @@
         <v>205</v>
       </c>
       <c r="B364" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C364">
         <v>0</v>
@@ -5953,7 +5953,7 @@
         <v>205</v>
       </c>
       <c r="B365" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C365">
         <v>0</v>
@@ -5964,7 +5964,7 @@
         <v>205</v>
       </c>
       <c r="B366" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C366">
         <v>0</v>
@@ -5975,7 +5975,7 @@
         <v>205</v>
       </c>
       <c r="B367" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C367">
         <v>0</v>
@@ -5986,7 +5986,7 @@
         <v>205</v>
       </c>
       <c r="B368" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C368">
         <v>0</v>
@@ -5997,7 +5997,7 @@
         <v>205</v>
       </c>
       <c r="B369" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C369">
         <v>0</v>
@@ -6008,7 +6008,7 @@
         <v>205</v>
       </c>
       <c r="B370" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C370">
         <v>0</v>
@@ -6019,7 +6019,7 @@
         <v>205</v>
       </c>
       <c r="B371" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C371">
         <v>0</v>
@@ -6030,7 +6030,7 @@
         <v>205</v>
       </c>
       <c r="B372" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C372">
         <v>0</v>
@@ -6041,7 +6041,7 @@
         <v>205</v>
       </c>
       <c r="B373" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C373">
         <v>0</v>
@@ -6052,7 +6052,7 @@
         <v>205</v>
       </c>
       <c r="B374" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C374">
         <v>0</v>
@@ -6063,7 +6063,7 @@
         <v>205</v>
       </c>
       <c r="B375" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C375">
         <v>0</v>
@@ -6074,7 +6074,7 @@
         <v>205</v>
       </c>
       <c r="B376" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C376">
         <v>0</v>
@@ -6085,7 +6085,7 @@
         <v>205</v>
       </c>
       <c r="B377" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C377">
         <v>0</v>
@@ -6096,7 +6096,7 @@
         <v>205</v>
       </c>
       <c r="B378" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C378">
         <v>0</v>
@@ -6107,10 +6107,10 @@
         <v>205</v>
       </c>
       <c r="B379" t="s">
-        <v>209</v>
+        <v>106</v>
       </c>
       <c r="C379">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="380" spans="1:3">
@@ -6118,10 +6118,10 @@
         <v>205</v>
       </c>
       <c r="B380" t="s">
-        <v>63</v>
+        <v>209</v>
       </c>
       <c r="C380">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="381" spans="1:3">
@@ -6129,7 +6129,7 @@
         <v>205</v>
       </c>
       <c r="B381" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C381">
         <v>0</v>
@@ -6140,7 +6140,7 @@
         <v>205</v>
       </c>
       <c r="B382" t="s">
-        <v>158</v>
+        <v>64</v>
       </c>
       <c r="C382">
         <v>0</v>
@@ -6151,7 +6151,7 @@
         <v>205</v>
       </c>
       <c r="B383" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C383">
         <v>0</v>
@@ -6162,7 +6162,7 @@
         <v>205</v>
       </c>
       <c r="B384" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C384">
         <v>0</v>
@@ -6173,7 +6173,7 @@
         <v>205</v>
       </c>
       <c r="B385" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C385">
         <v>0</v>
@@ -6184,7 +6184,7 @@
         <v>205</v>
       </c>
       <c r="B386" t="s">
-        <v>195</v>
+        <v>161</v>
       </c>
       <c r="C386">
         <v>0</v>
@@ -6195,13 +6195,10 @@
         <v>205</v>
       </c>
       <c r="B387" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="C387">
         <v>0</v>
-      </c>
-      <c r="D387">
-        <v>1</v>
       </c>
     </row>
     <row r="388" spans="1:4">
@@ -6209,10 +6206,13 @@
         <v>205</v>
       </c>
       <c r="B388" t="s">
-        <v>34</v>
+        <v>204</v>
       </c>
       <c r="C388">
         <v>0</v>
+      </c>
+      <c r="D388">
+        <v>1</v>
       </c>
     </row>
     <row r="389" spans="1:4">
@@ -6220,10 +6220,10 @@
         <v>205</v>
       </c>
       <c r="B389" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C389">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="390" spans="1:4">
@@ -6231,10 +6231,10 @@
         <v>205</v>
       </c>
       <c r="B390" t="s">
-        <v>117</v>
+        <v>35</v>
       </c>
       <c r="C390">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="391" spans="1:4">
@@ -6242,7 +6242,7 @@
         <v>205</v>
       </c>
       <c r="B391" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C391">
         <v>0</v>
@@ -6250,13 +6250,13 @@
     </row>
     <row r="392" spans="1:4">
       <c r="A392" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B392" t="s">
-        <v>5</v>
+        <v>118</v>
       </c>
       <c r="C392">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="393" spans="1:4">
@@ -6264,10 +6264,10 @@
         <v>210</v>
       </c>
       <c r="B393" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C393">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="394" spans="1:4">
@@ -6275,13 +6275,10 @@
         <v>210</v>
       </c>
       <c r="B394" t="s">
-        <v>211</v>
+        <v>6</v>
       </c>
       <c r="C394">
         <v>0</v>
-      </c>
-      <c r="D394">
-        <v>1</v>
       </c>
     </row>
     <row r="395" spans="1:4">
@@ -6289,7 +6286,7 @@
         <v>210</v>
       </c>
       <c r="B395" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C395">
         <v>0</v>
@@ -6303,7 +6300,7 @@
         <v>210</v>
       </c>
       <c r="B396" t="s">
-        <v>131</v>
+        <v>212</v>
       </c>
       <c r="C396">
         <v>0</v>
@@ -6317,7 +6314,7 @@
         <v>210</v>
       </c>
       <c r="B397" t="s">
-        <v>213</v>
+        <v>131</v>
       </c>
       <c r="C397">
         <v>0</v>
@@ -6331,7 +6328,7 @@
         <v>210</v>
       </c>
       <c r="B398" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C398">
         <v>0</v>
@@ -6345,7 +6342,7 @@
         <v>210</v>
       </c>
       <c r="B399" t="s">
-        <v>79</v>
+        <v>214</v>
       </c>
       <c r="C399">
         <v>0</v>
@@ -6359,7 +6356,7 @@
         <v>210</v>
       </c>
       <c r="B400" t="s">
-        <v>215</v>
+        <v>79</v>
       </c>
       <c r="C400">
         <v>0</v>
@@ -6373,7 +6370,7 @@
         <v>210</v>
       </c>
       <c r="B401" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C401">
         <v>0</v>
@@ -6387,10 +6384,13 @@
         <v>210</v>
       </c>
       <c r="B402" t="s">
-        <v>34</v>
+        <v>216</v>
       </c>
       <c r="C402">
         <v>0</v>
+      </c>
+      <c r="D402">
+        <v>1</v>
       </c>
     </row>
     <row r="403" spans="1:4">
@@ -6398,18 +6398,18 @@
         <v>210</v>
       </c>
       <c r="B403" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C403">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="404" spans="1:4">
       <c r="A404" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="B404" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="C404">
         <v>1</v>
@@ -6420,10 +6420,10 @@
         <v>217</v>
       </c>
       <c r="B405" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C405">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="406" spans="1:4">
@@ -6431,10 +6431,10 @@
         <v>217</v>
       </c>
       <c r="B406" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C406">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="407" spans="1:4">
@@ -6442,10 +6442,10 @@
         <v>217</v>
       </c>
       <c r="B407" t="s">
-        <v>136</v>
+        <v>25</v>
       </c>
       <c r="C407">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="408" spans="1:4">
@@ -6453,13 +6453,10 @@
         <v>217</v>
       </c>
       <c r="B408" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="C408">
         <v>0</v>
-      </c>
-      <c r="D408">
-        <v>1</v>
       </c>
     </row>
     <row r="409" spans="1:4">
@@ -6467,7 +6464,7 @@
         <v>217</v>
       </c>
       <c r="B409" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C409">
         <v>0</v>
@@ -6481,7 +6478,7 @@
         <v>217</v>
       </c>
       <c r="B410" t="s">
-        <v>141</v>
+        <v>64</v>
       </c>
       <c r="C410">
         <v>0</v>
@@ -6495,7 +6492,7 @@
         <v>217</v>
       </c>
       <c r="B411" t="s">
-        <v>218</v>
+        <v>141</v>
       </c>
       <c r="C411">
         <v>0</v>
@@ -6509,7 +6506,7 @@
         <v>217</v>
       </c>
       <c r="B412" t="s">
-        <v>164</v>
+        <v>218</v>
       </c>
       <c r="C412">
         <v>0</v>
@@ -6523,10 +6520,13 @@
         <v>217</v>
       </c>
       <c r="B413" t="s">
-        <v>219</v>
+        <v>164</v>
       </c>
       <c r="C413">
         <v>0</v>
+      </c>
+      <c r="D413">
+        <v>1</v>
       </c>
     </row>
     <row r="414" spans="1:4">
@@ -6534,13 +6534,10 @@
         <v>217</v>
       </c>
       <c r="B414" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C414">
         <v>0</v>
-      </c>
-      <c r="D414">
-        <v>1</v>
       </c>
     </row>
     <row r="415" spans="1:4">
@@ -6548,10 +6545,13 @@
         <v>217</v>
       </c>
       <c r="B415" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C415">
         <v>0</v>
+      </c>
+      <c r="D415">
+        <v>1</v>
       </c>
     </row>
     <row r="416" spans="1:4">
@@ -6559,13 +6559,10 @@
         <v>217</v>
       </c>
       <c r="B416" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C416">
         <v>0</v>
-      </c>
-      <c r="D416">
-        <v>1</v>
       </c>
     </row>
     <row r="417" spans="1:4">
@@ -6573,7 +6570,7 @@
         <v>217</v>
       </c>
       <c r="B417" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C417">
         <v>0</v>
@@ -6587,7 +6584,7 @@
         <v>217</v>
       </c>
       <c r="B418" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C418">
         <v>0</v>
@@ -6601,7 +6598,7 @@
         <v>217</v>
       </c>
       <c r="B419" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C419">
         <v>0</v>
@@ -6615,7 +6612,7 @@
         <v>217</v>
       </c>
       <c r="B420" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C420">
         <v>0</v>
@@ -6629,7 +6626,7 @@
         <v>217</v>
       </c>
       <c r="B421" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C421">
         <v>0</v>
@@ -6643,7 +6640,7 @@
         <v>217</v>
       </c>
       <c r="B422" t="s">
-        <v>33</v>
+        <v>227</v>
       </c>
       <c r="C422">
         <v>0</v>
@@ -6657,7 +6654,7 @@
         <v>217</v>
       </c>
       <c r="B423" t="s">
-        <v>228</v>
+        <v>33</v>
       </c>
       <c r="C423">
         <v>0</v>
@@ -6671,10 +6668,13 @@
         <v>217</v>
       </c>
       <c r="B424" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C424">
         <v>0</v>
+      </c>
+      <c r="D424">
+        <v>1</v>
       </c>
     </row>
     <row r="425" spans="1:4">
@@ -6682,7 +6682,7 @@
         <v>217</v>
       </c>
       <c r="B425" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C425">
         <v>0</v>
@@ -6693,13 +6693,10 @@
         <v>217</v>
       </c>
       <c r="B426" t="s">
-        <v>85</v>
+        <v>230</v>
       </c>
       <c r="C426">
         <v>0</v>
-      </c>
-      <c r="D426">
-        <v>1</v>
       </c>
     </row>
     <row r="427" spans="1:4">
@@ -6707,7 +6704,7 @@
         <v>217</v>
       </c>
       <c r="B427" t="s">
-        <v>231</v>
+        <v>85</v>
       </c>
       <c r="C427">
         <v>0</v>
@@ -6721,7 +6718,7 @@
         <v>217</v>
       </c>
       <c r="B428" t="s">
-        <v>202</v>
+        <v>231</v>
       </c>
       <c r="C428">
         <v>0</v>
@@ -6735,10 +6732,13 @@
         <v>217</v>
       </c>
       <c r="B429" t="s">
-        <v>232</v>
+        <v>202</v>
       </c>
       <c r="C429">
         <v>0</v>
+      </c>
+      <c r="D429">
+        <v>1</v>
       </c>
     </row>
     <row r="430" spans="1:4">
@@ -6746,7 +6746,7 @@
         <v>217</v>
       </c>
       <c r="B430" t="s">
-        <v>34</v>
+        <v>232</v>
       </c>
       <c r="C430">
         <v>0</v>
@@ -6757,13 +6757,10 @@
         <v>217</v>
       </c>
       <c r="B431" t="s">
-        <v>233</v>
+        <v>34</v>
       </c>
       <c r="C431">
         <v>0</v>
-      </c>
-      <c r="D431">
-        <v>1</v>
       </c>
     </row>
     <row r="432" spans="1:4">
@@ -6771,7 +6768,7 @@
         <v>217</v>
       </c>
       <c r="B432" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C432">
         <v>0</v>
@@ -6785,10 +6782,13 @@
         <v>217</v>
       </c>
       <c r="B433" t="s">
-        <v>23</v>
+        <v>234</v>
       </c>
       <c r="C433">
         <v>0</v>
+      </c>
+      <c r="D433">
+        <v>1</v>
       </c>
     </row>
     <row r="434" spans="1:4">
@@ -6796,7 +6796,7 @@
         <v>217</v>
       </c>
       <c r="B434" t="s">
-        <v>235</v>
+        <v>23</v>
       </c>
       <c r="C434">
         <v>0</v>
@@ -6807,23 +6807,23 @@
         <v>217</v>
       </c>
       <c r="B435" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C435">
         <v>0</v>
-      </c>
-      <c r="D435">
-        <v>1</v>
       </c>
     </row>
     <row r="436" spans="1:4">
       <c r="A436" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
       <c r="B436" t="s">
-        <v>5</v>
+        <v>236</v>
       </c>
       <c r="C436">
+        <v>0</v>
+      </c>
+      <c r="D436">
         <v>1</v>
       </c>
     </row>
@@ -6832,7 +6832,7 @@
         <v>237</v>
       </c>
       <c r="B437" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="C437">
         <v>1</v>
@@ -6843,10 +6843,10 @@
         <v>237</v>
       </c>
       <c r="B438" t="s">
-        <v>181</v>
+        <v>25</v>
       </c>
       <c r="C438">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="439" spans="1:4">
@@ -6854,10 +6854,10 @@
         <v>237</v>
       </c>
       <c r="B439" t="s">
-        <v>80</v>
+        <v>181</v>
       </c>
       <c r="C439">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="440" spans="1:4">
@@ -6865,10 +6865,10 @@
         <v>237</v>
       </c>
       <c r="B440" t="s">
-        <v>238</v>
+        <v>80</v>
       </c>
       <c r="C440">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="441" spans="1:4">
@@ -6876,13 +6876,10 @@
         <v>237</v>
       </c>
       <c r="B441" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C441">
         <v>0</v>
-      </c>
-      <c r="D441">
-        <v>1</v>
       </c>
     </row>
     <row r="442" spans="1:4">
@@ -6890,7 +6887,7 @@
         <v>237</v>
       </c>
       <c r="B442" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C442">
         <v>0</v>
@@ -6904,7 +6901,7 @@
         <v>237</v>
       </c>
       <c r="B443" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C443">
         <v>0</v>
@@ -6918,7 +6915,7 @@
         <v>237</v>
       </c>
       <c r="B444" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C444">
         <v>0</v>
@@ -6932,7 +6929,7 @@
         <v>237</v>
       </c>
       <c r="B445" t="s">
-        <v>120</v>
+        <v>242</v>
       </c>
       <c r="C445">
         <v>0</v>
@@ -6946,7 +6943,7 @@
         <v>237</v>
       </c>
       <c r="B446" t="s">
-        <v>243</v>
+        <v>120</v>
       </c>
       <c r="C446">
         <v>0</v>
@@ -6960,7 +6957,7 @@
         <v>237</v>
       </c>
       <c r="B447" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C447">
         <v>0</v>
@@ -6974,7 +6971,7 @@
         <v>237</v>
       </c>
       <c r="B448" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C448">
         <v>0</v>
@@ -6988,7 +6985,7 @@
         <v>237</v>
       </c>
       <c r="B449" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C449">
         <v>0</v>
@@ -7002,7 +6999,7 @@
         <v>237</v>
       </c>
       <c r="B450" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C450">
         <v>0</v>
@@ -7016,7 +7013,7 @@
         <v>237</v>
       </c>
       <c r="B451" t="s">
-        <v>33</v>
+        <v>247</v>
       </c>
       <c r="C451">
         <v>0</v>
@@ -7030,7 +7027,7 @@
         <v>237</v>
       </c>
       <c r="B452" t="s">
-        <v>248</v>
+        <v>33</v>
       </c>
       <c r="C452">
         <v>0</v>
@@ -7044,7 +7041,7 @@
         <v>237</v>
       </c>
       <c r="B453" t="s">
-        <v>85</v>
+        <v>248</v>
       </c>
       <c r="C453">
         <v>0</v>
@@ -7058,7 +7055,7 @@
         <v>237</v>
       </c>
       <c r="B454" t="s">
-        <v>231</v>
+        <v>85</v>
       </c>
       <c r="C454">
         <v>0</v>
@@ -7072,7 +7069,7 @@
         <v>237</v>
       </c>
       <c r="B455" t="s">
-        <v>202</v>
+        <v>231</v>
       </c>
       <c r="C455">
         <v>0</v>
@@ -7086,10 +7083,13 @@
         <v>237</v>
       </c>
       <c r="B456" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="C456">
         <v>0</v>
+      </c>
+      <c r="D456">
+        <v>1</v>
       </c>
     </row>
     <row r="457" spans="1:4">
@@ -7097,7 +7097,7 @@
         <v>237</v>
       </c>
       <c r="B457" t="s">
-        <v>63</v>
+        <v>194</v>
       </c>
       <c r="C457">
         <v>0</v>
@@ -7108,7 +7108,7 @@
         <v>237</v>
       </c>
       <c r="B458" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C458">
         <v>0</v>
@@ -7116,16 +7116,13 @@
     </row>
     <row r="459" spans="1:4">
       <c r="A459" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="B459" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="C459">
         <v>0</v>
-      </c>
-      <c r="D459">
-        <v>1</v>
       </c>
     </row>
     <row r="460" spans="1:4">
@@ -7133,9 +7130,12 @@
         <v>249</v>
       </c>
       <c r="B460" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C460">
+        <v>0</v>
+      </c>
+      <c r="D460">
         <v>1</v>
       </c>
     </row>
@@ -7144,7 +7144,7 @@
         <v>249</v>
       </c>
       <c r="B461" t="s">
-        <v>71</v>
+        <v>5</v>
       </c>
       <c r="C461">
         <v>1</v>
@@ -7155,10 +7155,10 @@
         <v>249</v>
       </c>
       <c r="B462" t="s">
-        <v>250</v>
+        <v>71</v>
       </c>
       <c r="C462">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="463" spans="1:4">
@@ -7166,7 +7166,7 @@
         <v>249</v>
       </c>
       <c r="B463" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C463">
         <v>0</v>
@@ -7177,7 +7177,7 @@
         <v>249</v>
       </c>
       <c r="B464" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C464">
         <v>0</v>
@@ -7188,7 +7188,7 @@
         <v>249</v>
       </c>
       <c r="B465" t="s">
-        <v>112</v>
+        <v>252</v>
       </c>
       <c r="C465">
         <v>0</v>
@@ -7199,7 +7199,7 @@
         <v>249</v>
       </c>
       <c r="B466" t="s">
-        <v>253</v>
+        <v>112</v>
       </c>
       <c r="C466">
         <v>0</v>
@@ -7210,10 +7210,10 @@
         <v>249</v>
       </c>
       <c r="B467" t="s">
-        <v>70</v>
+        <v>253</v>
       </c>
       <c r="C467">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="468" spans="1:4">
@@ -7221,10 +7221,10 @@
         <v>249</v>
       </c>
       <c r="B468" t="s">
-        <v>116</v>
+        <v>70</v>
       </c>
       <c r="C468">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="469" spans="1:4">
@@ -7232,7 +7232,7 @@
         <v>249</v>
       </c>
       <c r="B469" t="s">
-        <v>6</v>
+        <v>116</v>
       </c>
       <c r="C469">
         <v>0</v>
@@ -7243,7 +7243,7 @@
         <v>249</v>
       </c>
       <c r="B470" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
       <c r="C470">
         <v>0</v>
@@ -7254,7 +7254,7 @@
         <v>249</v>
       </c>
       <c r="B471" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C471">
         <v>0</v>
@@ -7265,7 +7265,7 @@
         <v>249</v>
       </c>
       <c r="B472" t="s">
-        <v>254</v>
+        <v>64</v>
       </c>
       <c r="C472">
         <v>0</v>
@@ -7276,13 +7276,10 @@
         <v>249</v>
       </c>
       <c r="B473" t="s">
-        <v>225</v>
+        <v>254</v>
       </c>
       <c r="C473">
         <v>0</v>
-      </c>
-      <c r="D473">
-        <v>1</v>
       </c>
     </row>
     <row r="474" spans="1:4">
@@ -7290,7 +7287,7 @@
         <v>249</v>
       </c>
       <c r="B474" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C474">
         <v>0</v>
@@ -7304,7 +7301,7 @@
         <v>249</v>
       </c>
       <c r="B475" t="s">
-        <v>255</v>
+        <v>226</v>
       </c>
       <c r="C475">
         <v>0</v>
@@ -7318,7 +7315,7 @@
         <v>249</v>
       </c>
       <c r="B476" t="s">
-        <v>86</v>
+        <v>255</v>
       </c>
       <c r="C476">
         <v>0</v>
@@ -7332,10 +7329,13 @@
         <v>249</v>
       </c>
       <c r="B477" t="s">
-        <v>256</v>
+        <v>86</v>
       </c>
       <c r="C477">
         <v>0</v>
+      </c>
+      <c r="D477">
+        <v>1</v>
       </c>
     </row>
     <row r="478" spans="1:4">
@@ -7343,7 +7343,7 @@
         <v>249</v>
       </c>
       <c r="B478" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C478">
         <v>0</v>
@@ -7354,7 +7354,7 @@
         <v>249</v>
       </c>
       <c r="B479" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C479">
         <v>0</v>
@@ -7365,13 +7365,10 @@
         <v>249</v>
       </c>
       <c r="B480" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C480">
         <v>0</v>
-      </c>
-      <c r="D480">
-        <v>1</v>
       </c>
     </row>
     <row r="481" spans="1:4">
@@ -7379,7 +7376,7 @@
         <v>249</v>
       </c>
       <c r="B481" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C481">
         <v>0</v>
@@ -7393,10 +7390,13 @@
         <v>249</v>
       </c>
       <c r="B482" t="s">
-        <v>109</v>
+        <v>260</v>
       </c>
       <c r="C482">
         <v>0</v>
+      </c>
+      <c r="D482">
+        <v>1</v>
       </c>
     </row>
     <row r="483" spans="1:4">
@@ -7404,7 +7404,7 @@
         <v>249</v>
       </c>
       <c r="B483" t="s">
-        <v>261</v>
+        <v>109</v>
       </c>
       <c r="C483">
         <v>0</v>
@@ -7415,7 +7415,7 @@
         <v>249</v>
       </c>
       <c r="B484" t="s">
-        <v>281</v>
+        <v>261</v>
       </c>
       <c r="C484">
         <v>0</v>
@@ -7426,7 +7426,7 @@
         <v>249</v>
       </c>
       <c r="B485" t="s">
-        <v>262</v>
+        <v>281</v>
       </c>
       <c r="C485">
         <v>0</v>
@@ -7437,7 +7437,7 @@
         <v>249</v>
       </c>
       <c r="B486" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C486">
         <v>0</v>
@@ -7448,7 +7448,7 @@
         <v>249</v>
       </c>
       <c r="B487" t="s">
-        <v>110</v>
+        <v>263</v>
       </c>
       <c r="C487">
         <v>0</v>
@@ -7459,7 +7459,7 @@
         <v>249</v>
       </c>
       <c r="B488" t="s">
-        <v>264</v>
+        <v>110</v>
       </c>
       <c r="C488">
         <v>0</v>
@@ -7470,7 +7470,7 @@
         <v>249</v>
       </c>
       <c r="B489" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C489">
         <v>0</v>
@@ -7481,7 +7481,7 @@
         <v>249</v>
       </c>
       <c r="B490" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C490">
         <v>0</v>
@@ -7492,7 +7492,7 @@
         <v>249</v>
       </c>
       <c r="B491" t="s">
-        <v>126</v>
+        <v>266</v>
       </c>
       <c r="C491">
         <v>0</v>
@@ -7503,7 +7503,7 @@
         <v>249</v>
       </c>
       <c r="B492" t="s">
-        <v>267</v>
+        <v>126</v>
       </c>
       <c r="C492">
         <v>0</v>
@@ -7514,7 +7514,7 @@
         <v>249</v>
       </c>
       <c r="B493" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C493">
         <v>0</v>
@@ -7525,13 +7525,10 @@
         <v>249</v>
       </c>
       <c r="B494" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C494">
         <v>0</v>
-      </c>
-      <c r="D494">
-        <v>1</v>
       </c>
     </row>
     <row r="495" spans="1:4">
@@ -7539,7 +7536,7 @@
         <v>249</v>
       </c>
       <c r="B495" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C495">
         <v>0</v>
@@ -7553,10 +7550,13 @@
         <v>249</v>
       </c>
       <c r="B496" t="s">
-        <v>76</v>
+        <v>270</v>
       </c>
       <c r="C496">
         <v>0</v>
+      </c>
+      <c r="D496">
+        <v>1</v>
       </c>
     </row>
     <row r="497" spans="1:4">
@@ -7564,7 +7564,7 @@
         <v>249</v>
       </c>
       <c r="B497" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C497">
         <v>0</v>
@@ -7575,7 +7575,7 @@
         <v>249</v>
       </c>
       <c r="B498" t="s">
-        <v>271</v>
+        <v>77</v>
       </c>
       <c r="C498">
         <v>0</v>
@@ -7586,13 +7586,10 @@
         <v>249</v>
       </c>
       <c r="B499" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C499">
         <v>0</v>
-      </c>
-      <c r="D499">
-        <v>1</v>
       </c>
     </row>
     <row r="500" spans="1:4">
@@ -7600,10 +7597,13 @@
         <v>249</v>
       </c>
       <c r="B500" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C500">
         <v>0</v>
+      </c>
+      <c r="D500">
+        <v>1</v>
       </c>
     </row>
     <row r="501" spans="1:4">
@@ -7611,7 +7611,7 @@
         <v>249</v>
       </c>
       <c r="B501" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C501">
         <v>0</v>
@@ -7622,7 +7622,7 @@
         <v>249</v>
       </c>
       <c r="B502" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C502">
         <v>0</v>
@@ -7633,7 +7633,7 @@
         <v>249</v>
       </c>
       <c r="B503" t="s">
-        <v>124</v>
+        <v>275</v>
       </c>
       <c r="C503">
         <v>0</v>
@@ -7644,7 +7644,7 @@
         <v>249</v>
       </c>
       <c r="B504" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C504">
         <v>0</v>
@@ -7655,7 +7655,7 @@
         <v>249</v>
       </c>
       <c r="B505" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C505">
         <v>0</v>
@@ -7666,7 +7666,7 @@
         <v>249</v>
       </c>
       <c r="B506" t="s">
-        <v>276</v>
+        <v>119</v>
       </c>
       <c r="C506">
         <v>0</v>
@@ -7677,13 +7677,10 @@
         <v>249</v>
       </c>
       <c r="B507" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C507">
         <v>0</v>
-      </c>
-      <c r="D507">
-        <v>1</v>
       </c>
     </row>
     <row r="508" spans="1:4">
@@ -7691,7 +7688,7 @@
         <v>249</v>
       </c>
       <c r="B508" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C508">
         <v>0</v>
@@ -7705,10 +7702,13 @@
         <v>249</v>
       </c>
       <c r="B509" t="s">
-        <v>34</v>
+        <v>278</v>
       </c>
       <c r="C509">
         <v>0</v>
+      </c>
+      <c r="D509">
+        <v>1</v>
       </c>
     </row>
     <row r="510" spans="1:4">
@@ -7716,7 +7716,7 @@
         <v>249</v>
       </c>
       <c r="B510" t="s">
-        <v>339</v>
+        <v>34</v>
       </c>
       <c r="C510">
         <v>0</v>
@@ -7724,13 +7724,13 @@
     </row>
     <row r="511" spans="1:4">
       <c r="A511" t="s">
-        <v>279</v>
+        <v>249</v>
       </c>
       <c r="B511" t="s">
-        <v>5</v>
+        <v>339</v>
       </c>
       <c r="C511">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="512" spans="1:4">
@@ -7738,7 +7738,7 @@
         <v>279</v>
       </c>
       <c r="B512" t="s">
-        <v>69</v>
+        <v>5</v>
       </c>
       <c r="C512">
         <v>1</v>
@@ -7749,10 +7749,10 @@
         <v>279</v>
       </c>
       <c r="B513" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C513">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="514" spans="1:3">
@@ -7760,7 +7760,7 @@
         <v>279</v>
       </c>
       <c r="B514" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C514">
         <v>0</v>
@@ -7771,7 +7771,7 @@
         <v>279</v>
       </c>
       <c r="B515" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C515">
         <v>0</v>
@@ -7782,7 +7782,7 @@
         <v>279</v>
       </c>
       <c r="B516" t="s">
-        <v>280</v>
+        <v>66</v>
       </c>
       <c r="C516">
         <v>0</v>
@@ -7793,7 +7793,7 @@
         <v>279</v>
       </c>
       <c r="B517" t="s">
-        <v>109</v>
+        <v>280</v>
       </c>
       <c r="C517">
         <v>0</v>
@@ -7804,7 +7804,7 @@
         <v>279</v>
       </c>
       <c r="B518" t="s">
-        <v>261</v>
+        <v>109</v>
       </c>
       <c r="C518">
         <v>0</v>
@@ -7815,7 +7815,7 @@
         <v>279</v>
       </c>
       <c r="B519" t="s">
-        <v>281</v>
+        <v>261</v>
       </c>
       <c r="C519">
         <v>0</v>
@@ -7826,7 +7826,7 @@
         <v>279</v>
       </c>
       <c r="B520" t="s">
-        <v>262</v>
+        <v>281</v>
       </c>
       <c r="C520">
         <v>0</v>
@@ -7837,7 +7837,7 @@
         <v>279</v>
       </c>
       <c r="B521" t="s">
-        <v>282</v>
+        <v>262</v>
       </c>
       <c r="C521">
         <v>0</v>
@@ -7848,7 +7848,7 @@
         <v>279</v>
       </c>
       <c r="B522" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C522">
         <v>0</v>
@@ -7859,7 +7859,7 @@
         <v>279</v>
       </c>
       <c r="B523" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C523">
         <v>0</v>
@@ -7870,7 +7870,7 @@
         <v>279</v>
       </c>
       <c r="B524" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C524">
         <v>0</v>
@@ -7881,7 +7881,7 @@
         <v>279</v>
       </c>
       <c r="B525" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C525">
         <v>0</v>
@@ -7892,7 +7892,7 @@
         <v>279</v>
       </c>
       <c r="B526" t="s">
-        <v>67</v>
+        <v>286</v>
       </c>
       <c r="C526">
         <v>0</v>
@@ -7903,7 +7903,7 @@
         <v>279</v>
       </c>
       <c r="B527" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
       <c r="C527">
         <v>0</v>
@@ -7914,7 +7914,7 @@
         <v>279</v>
       </c>
       <c r="B528" t="s">
-        <v>264</v>
+        <v>110</v>
       </c>
       <c r="C528">
         <v>0</v>
@@ -7925,7 +7925,7 @@
         <v>279</v>
       </c>
       <c r="B529" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C529">
         <v>0</v>
@@ -7936,7 +7936,7 @@
         <v>279</v>
       </c>
       <c r="B530" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C530">
         <v>0</v>
@@ -7947,7 +7947,7 @@
         <v>279</v>
       </c>
       <c r="B531" t="s">
-        <v>287</v>
+        <v>266</v>
       </c>
       <c r="C531">
         <v>0</v>
@@ -7958,7 +7958,7 @@
         <v>279</v>
       </c>
       <c r="B532" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C532">
         <v>0</v>
@@ -7969,7 +7969,7 @@
         <v>279</v>
       </c>
       <c r="B533" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C533">
         <v>0</v>
@@ -7980,7 +7980,7 @@
         <v>279</v>
       </c>
       <c r="B534" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C534">
         <v>0</v>
@@ -7991,7 +7991,7 @@
         <v>279</v>
       </c>
       <c r="B535" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C535">
         <v>0</v>
@@ -8002,7 +8002,7 @@
         <v>279</v>
       </c>
       <c r="B536" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C536">
         <v>0</v>
@@ -8013,13 +8013,10 @@
         <v>279</v>
       </c>
       <c r="B537" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C537">
         <v>0</v>
-      </c>
-      <c r="D537">
-        <v>1</v>
       </c>
     </row>
     <row r="538" spans="1:4">
@@ -8027,7 +8024,7 @@
         <v>279</v>
       </c>
       <c r="B538" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C538">
         <v>0</v>
@@ -8041,24 +8038,24 @@
         <v>279</v>
       </c>
       <c r="B539" t="s">
-        <v>126</v>
+        <v>294</v>
       </c>
       <c r="C539">
         <v>0</v>
+      </c>
+      <c r="D539">
+        <v>1</v>
       </c>
     </row>
     <row r="540" spans="1:4">
       <c r="A540" t="s">
-        <v>295</v>
+        <v>279</v>
       </c>
       <c r="B540" t="s">
-        <v>33</v>
+        <v>126</v>
       </c>
       <c r="C540">
         <v>0</v>
-      </c>
-      <c r="D540">
-        <v>1</v>
       </c>
     </row>
     <row r="541" spans="1:4">
@@ -8066,9 +8063,12 @@
         <v>295</v>
       </c>
       <c r="B541" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C541">
+        <v>0</v>
+      </c>
+      <c r="D541">
         <v>1</v>
       </c>
     </row>
@@ -8077,10 +8077,10 @@
         <v>295</v>
       </c>
       <c r="B542" t="s">
-        <v>112</v>
+        <v>5</v>
       </c>
       <c r="C542">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="543" spans="1:4">
@@ -8088,10 +8088,10 @@
         <v>295</v>
       </c>
       <c r="B543" t="s">
-        <v>71</v>
+        <v>112</v>
       </c>
       <c r="C543">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="544" spans="1:4">
@@ -8099,10 +8099,10 @@
         <v>295</v>
       </c>
       <c r="B544" t="s">
-        <v>251</v>
+        <v>71</v>
       </c>
       <c r="C544">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="545" spans="1:4">
@@ -8110,13 +8110,10 @@
         <v>295</v>
       </c>
       <c r="B545" t="s">
-        <v>120</v>
+        <v>251</v>
       </c>
       <c r="C545">
         <v>0</v>
-      </c>
-      <c r="D545">
-        <v>1</v>
       </c>
     </row>
     <row r="546" spans="1:4">
@@ -8124,7 +8121,7 @@
         <v>295</v>
       </c>
       <c r="B546" t="s">
-        <v>225</v>
+        <v>120</v>
       </c>
       <c r="C546">
         <v>0</v>
@@ -8138,10 +8135,13 @@
         <v>295</v>
       </c>
       <c r="B547" t="s">
-        <v>256</v>
+        <v>225</v>
       </c>
       <c r="C547">
         <v>0</v>
+      </c>
+      <c r="D547">
+        <v>1</v>
       </c>
     </row>
     <row r="548" spans="1:4">
@@ -8149,10 +8149,10 @@
         <v>295</v>
       </c>
       <c r="B548" t="s">
-        <v>80</v>
+        <v>256</v>
       </c>
       <c r="C548">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="549" spans="1:4">
@@ -8160,12 +8160,9 @@
         <v>295</v>
       </c>
       <c r="B549" t="s">
-        <v>296</v>
+        <v>80</v>
       </c>
       <c r="C549">
-        <v>0</v>
-      </c>
-      <c r="D549">
         <v>1</v>
       </c>
     </row>
@@ -8174,7 +8171,7 @@
         <v>295</v>
       </c>
       <c r="B550" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C550">
         <v>0</v>
@@ -8188,7 +8185,7 @@
         <v>295</v>
       </c>
       <c r="B551" t="s">
-        <v>106</v>
+        <v>297</v>
       </c>
       <c r="C551">
         <v>0</v>
@@ -8202,7 +8199,7 @@
         <v>295</v>
       </c>
       <c r="B552" t="s">
-        <v>255</v>
+        <v>106</v>
       </c>
       <c r="C552">
         <v>0</v>
@@ -8216,7 +8213,7 @@
         <v>295</v>
       </c>
       <c r="B553" t="s">
-        <v>86</v>
+        <v>255</v>
       </c>
       <c r="C553">
         <v>0</v>
@@ -8230,10 +8227,13 @@
         <v>295</v>
       </c>
       <c r="B554" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C554">
         <v>0</v>
+      </c>
+      <c r="D554">
+        <v>1</v>
       </c>
     </row>
     <row r="555" spans="1:4">
@@ -8241,7 +8241,7 @@
         <v>295</v>
       </c>
       <c r="B555" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C555">
         <v>0</v>
@@ -8252,7 +8252,7 @@
         <v>295</v>
       </c>
       <c r="B556" t="s">
-        <v>298</v>
+        <v>126</v>
       </c>
       <c r="C556">
         <v>0</v>
@@ -8263,7 +8263,7 @@
         <v>295</v>
       </c>
       <c r="B557" t="s">
-        <v>54</v>
+        <v>298</v>
       </c>
       <c r="C557">
         <v>0</v>
@@ -8274,7 +8274,7 @@
         <v>295</v>
       </c>
       <c r="B558" t="s">
-        <v>299</v>
+        <v>54</v>
       </c>
       <c r="C558">
         <v>0</v>
@@ -8285,7 +8285,7 @@
         <v>295</v>
       </c>
       <c r="B559" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C559">
         <v>0</v>
@@ -8296,7 +8296,7 @@
         <v>295</v>
       </c>
       <c r="B560" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C560">
         <v>0</v>
@@ -8307,13 +8307,10 @@
         <v>295</v>
       </c>
       <c r="B561" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C561">
         <v>0</v>
-      </c>
-      <c r="D561">
-        <v>1</v>
       </c>
     </row>
     <row r="562" spans="1:4">
@@ -8321,7 +8318,7 @@
         <v>295</v>
       </c>
       <c r="B562" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C562">
         <v>0</v>
@@ -8335,7 +8332,7 @@
         <v>295</v>
       </c>
       <c r="B563" t="s">
-        <v>89</v>
+        <v>303</v>
       </c>
       <c r="C563">
         <v>0</v>
@@ -8349,7 +8346,7 @@
         <v>295</v>
       </c>
       <c r="B564" t="s">
-        <v>304</v>
+        <v>89</v>
       </c>
       <c r="C564">
         <v>0</v>
@@ -8363,10 +8360,13 @@
         <v>295</v>
       </c>
       <c r="B565" t="s">
-        <v>6</v>
+        <v>304</v>
       </c>
       <c r="C565">
         <v>0</v>
+      </c>
+      <c r="D565">
+        <v>1</v>
       </c>
     </row>
     <row r="566" spans="1:4">
@@ -8374,7 +8374,7 @@
         <v>295</v>
       </c>
       <c r="B566" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="C566">
         <v>0</v>
@@ -8385,7 +8385,7 @@
         <v>295</v>
       </c>
       <c r="B567" t="s">
-        <v>305</v>
+        <v>34</v>
       </c>
       <c r="C567">
         <v>0</v>
@@ -8396,7 +8396,7 @@
         <v>295</v>
       </c>
       <c r="B568" t="s">
-        <v>69</v>
+        <v>305</v>
       </c>
       <c r="C568">
         <v>0</v>
@@ -8407,10 +8407,10 @@
         <v>295</v>
       </c>
       <c r="B569" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C569">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="570" spans="1:4">
@@ -8418,10 +8418,10 @@
         <v>295</v>
       </c>
       <c r="B570" t="s">
-        <v>306</v>
+        <v>70</v>
       </c>
       <c r="C570">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="571" spans="1:4">
@@ -8429,7 +8429,7 @@
         <v>295</v>
       </c>
       <c r="B571" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C571">
         <v>0</v>
@@ -8440,7 +8440,7 @@
         <v>295</v>
       </c>
       <c r="B572" t="s">
-        <v>257</v>
+        <v>307</v>
       </c>
       <c r="C572">
         <v>0</v>
@@ -8451,13 +8451,10 @@
         <v>295</v>
       </c>
       <c r="B573" t="s">
-        <v>78</v>
+        <v>257</v>
       </c>
       <c r="C573">
         <v>0</v>
-      </c>
-      <c r="D573">
-        <v>1</v>
       </c>
     </row>
     <row r="574" spans="1:4">
@@ -8465,10 +8462,13 @@
         <v>295</v>
       </c>
       <c r="B574" t="s">
-        <v>334</v>
+        <v>78</v>
       </c>
       <c r="C574">
         <v>0</v>
+      </c>
+      <c r="D574">
+        <v>1</v>
       </c>
     </row>
     <row r="575" spans="1:4">
@@ -8476,23 +8476,20 @@
         <v>295</v>
       </c>
       <c r="B575" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C575">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="576" spans="1:4">
       <c r="A576" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
       <c r="B576" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="C576">
-        <v>0</v>
-      </c>
-      <c r="D576">
         <v>1</v>
       </c>
     </row>
@@ -8501,9 +8498,12 @@
         <v>308</v>
       </c>
       <c r="B577" t="s">
-        <v>5</v>
+        <v>331</v>
       </c>
       <c r="C577">
+        <v>0</v>
+      </c>
+      <c r="D577">
         <v>1</v>
       </c>
     </row>
@@ -8512,7 +8512,7 @@
         <v>308</v>
       </c>
       <c r="B578" t="s">
-        <v>71</v>
+        <v>5</v>
       </c>
       <c r="C578">
         <v>1</v>
@@ -8523,10 +8523,10 @@
         <v>308</v>
       </c>
       <c r="B579" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C579">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="580" spans="1:4">
@@ -8534,10 +8534,10 @@
         <v>308</v>
       </c>
       <c r="B580" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C580">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="581" spans="1:4">
@@ -8545,7 +8545,7 @@
         <v>308</v>
       </c>
       <c r="B581" t="s">
-        <v>309</v>
+        <v>70</v>
       </c>
       <c r="C581">
         <v>1</v>
@@ -8556,7 +8556,7 @@
         <v>308</v>
       </c>
       <c r="B582" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C582">
         <v>1</v>
@@ -8567,10 +8567,10 @@
         <v>308</v>
       </c>
       <c r="B583" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C583">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="584" spans="1:4">
@@ -8578,7 +8578,7 @@
         <v>308</v>
       </c>
       <c r="B584" t="s">
-        <v>50</v>
+        <v>311</v>
       </c>
       <c r="C584">
         <v>0</v>
@@ -8589,7 +8589,7 @@
         <v>308</v>
       </c>
       <c r="B585" t="s">
-        <v>312</v>
+        <v>50</v>
       </c>
       <c r="C585">
         <v>0</v>
@@ -8600,13 +8600,10 @@
         <v>308</v>
       </c>
       <c r="B586" t="s">
-        <v>55</v>
+        <v>312</v>
       </c>
       <c r="C586">
         <v>0</v>
-      </c>
-      <c r="D586">
-        <v>1</v>
       </c>
     </row>
     <row r="587" spans="1:4">
@@ -8614,7 +8611,7 @@
         <v>308</v>
       </c>
       <c r="B587" t="s">
-        <v>313</v>
+        <v>55</v>
       </c>
       <c r="C587">
         <v>0</v>
@@ -8628,10 +8625,13 @@
         <v>308</v>
       </c>
       <c r="B588" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C588">
         <v>0</v>
+      </c>
+      <c r="D588">
+        <v>1</v>
       </c>
     </row>
     <row r="589" spans="1:4">
@@ -8639,13 +8639,10 @@
         <v>308</v>
       </c>
       <c r="B589" t="s">
-        <v>221</v>
+        <v>314</v>
       </c>
       <c r="C589">
         <v>0</v>
-      </c>
-      <c r="D589">
-        <v>1</v>
       </c>
     </row>
     <row r="590" spans="1:4">
@@ -8653,10 +8650,13 @@
         <v>308</v>
       </c>
       <c r="B590" t="s">
-        <v>112</v>
+        <v>221</v>
       </c>
       <c r="C590">
         <v>0</v>
+      </c>
+      <c r="D590">
+        <v>1</v>
       </c>
     </row>
     <row r="591" spans="1:4">
@@ -8664,13 +8664,10 @@
         <v>308</v>
       </c>
       <c r="B591" t="s">
-        <v>315</v>
+        <v>112</v>
       </c>
       <c r="C591">
         <v>0</v>
-      </c>
-      <c r="D591">
-        <v>1</v>
       </c>
     </row>
     <row r="592" spans="1:4">
@@ -8678,7 +8675,7 @@
         <v>308</v>
       </c>
       <c r="B592" t="s">
-        <v>18</v>
+        <v>315</v>
       </c>
       <c r="C592">
         <v>0</v>
@@ -8692,7 +8689,7 @@
         <v>308</v>
       </c>
       <c r="B593" t="s">
-        <v>316</v>
+        <v>18</v>
       </c>
       <c r="C593">
         <v>0</v>
@@ -8706,7 +8703,7 @@
         <v>308</v>
       </c>
       <c r="B594" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C594">
         <v>0</v>
@@ -8720,10 +8717,13 @@
         <v>308</v>
       </c>
       <c r="B595" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C595">
         <v>0</v>
+      </c>
+      <c r="D595">
+        <v>1</v>
       </c>
     </row>
     <row r="596" spans="1:4">
@@ -8731,13 +8731,10 @@
         <v>308</v>
       </c>
       <c r="B596" t="s">
-        <v>303</v>
+        <v>318</v>
       </c>
       <c r="C596">
         <v>0</v>
-      </c>
-      <c r="D596">
-        <v>1</v>
       </c>
     </row>
     <row r="597" spans="1:4">
@@ -8745,10 +8742,13 @@
         <v>308</v>
       </c>
       <c r="B597" t="s">
-        <v>319</v>
+        <v>303</v>
       </c>
       <c r="C597">
         <v>0</v>
+      </c>
+      <c r="D597">
+        <v>1</v>
       </c>
     </row>
     <row r="598" spans="1:4">
@@ -8756,7 +8756,7 @@
         <v>308</v>
       </c>
       <c r="B598" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C598">
         <v>0</v>
@@ -8767,7 +8767,7 @@
         <v>308</v>
       </c>
       <c r="B599" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C599">
         <v>0</v>
@@ -8778,7 +8778,7 @@
         <v>308</v>
       </c>
       <c r="B600" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C600">
         <v>0</v>
@@ -8789,7 +8789,7 @@
         <v>308</v>
       </c>
       <c r="B601" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C601">
         <v>0</v>
@@ -8800,7 +8800,7 @@
         <v>308</v>
       </c>
       <c r="B602" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C602">
         <v>0</v>
@@ -8811,7 +8811,7 @@
         <v>308</v>
       </c>
       <c r="B603" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C603">
         <v>0</v>
@@ -8822,7 +8822,7 @@
         <v>308</v>
       </c>
       <c r="B604" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C604">
         <v>0</v>
@@ -8833,7 +8833,7 @@
         <v>308</v>
       </c>
       <c r="B605" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C605">
         <v>0</v>
@@ -8844,7 +8844,7 @@
         <v>308</v>
       </c>
       <c r="B606" t="s">
-        <v>51</v>
+        <v>327</v>
       </c>
       <c r="C606">
         <v>0</v>
@@ -8855,7 +8855,7 @@
         <v>308</v>
       </c>
       <c r="B607" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C607">
         <v>0</v>
@@ -8866,7 +8866,7 @@
         <v>308</v>
       </c>
       <c r="B608" t="s">
-        <v>328</v>
+        <v>52</v>
       </c>
       <c r="C608">
         <v>0</v>
@@ -8877,44 +8877,44 @@
         <v>308</v>
       </c>
       <c r="B609" t="s">
+        <v>328</v>
+      </c>
+      <c r="C609">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="610" spans="1:4">
+      <c r="A610" t="s">
+        <v>308</v>
+      </c>
+      <c r="B610" t="s">
         <v>329</v>
       </c>
-      <c r="C609">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="610" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A610" s="3" t="s">
+      <c r="C610">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="611" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A611" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="B610" s="3" t="s">
+      <c r="B611" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="C610" s="3">
-        <v>0</v>
-      </c>
-      <c r="D610" s="3"/>
-    </row>
-    <row r="611" spans="1:4" ht="15.75" thickTop="1">
-      <c r="A611" t="s">
-        <v>350</v>
-      </c>
-      <c r="B611" t="s">
-        <v>5</v>
-      </c>
-      <c r="C611">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="612" spans="1:4">
+      <c r="C611" s="3">
+        <v>0</v>
+      </c>
+      <c r="D611" s="3"/>
+    </row>
+    <row r="612" spans="1:4" ht="15.75" thickTop="1">
       <c r="A612" t="s">
         <v>350</v>
       </c>
       <c r="B612" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C612">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="613" spans="1:4">
@@ -8922,7 +8922,7 @@
         <v>350</v>
       </c>
       <c r="B613" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C613">
         <v>0</v>
@@ -8933,7 +8933,7 @@
         <v>350</v>
       </c>
       <c r="B614" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="C614">
         <v>0</v>
@@ -8944,7 +8944,7 @@
         <v>350</v>
       </c>
       <c r="B615" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="C615">
         <v>0</v>
@@ -8955,7 +8955,7 @@
         <v>350</v>
       </c>
       <c r="B616" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="C616">
         <v>0</v>
@@ -8966,7 +8966,7 @@
         <v>350</v>
       </c>
       <c r="B617" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C617">
         <v>0</v>
@@ -8977,7 +8977,7 @@
         <v>350</v>
       </c>
       <c r="B618" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="C618">
         <v>0</v>
@@ -8988,7 +8988,7 @@
         <v>350</v>
       </c>
       <c r="B619" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C619">
         <v>0</v>
@@ -8999,7 +8999,7 @@
         <v>350</v>
       </c>
       <c r="B620" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C620">
         <v>0</v>
@@ -9010,7 +9010,7 @@
         <v>350</v>
       </c>
       <c r="B621" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C621">
         <v>0</v>
@@ -9021,7 +9021,7 @@
         <v>350</v>
       </c>
       <c r="B622" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="C622">
         <v>0</v>
@@ -9032,7 +9032,7 @@
         <v>350</v>
       </c>
       <c r="B623" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C623">
         <v>0</v>
@@ -9043,7 +9043,7 @@
         <v>350</v>
       </c>
       <c r="B624" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C624">
         <v>0</v>
@@ -9054,7 +9054,7 @@
         <v>350</v>
       </c>
       <c r="B625" t="s">
-        <v>351</v>
+        <v>52</v>
       </c>
       <c r="C625">
         <v>0</v>
@@ -9065,7 +9065,7 @@
         <v>350</v>
       </c>
       <c r="B626" t="s">
-        <v>21</v>
+        <v>351</v>
       </c>
       <c r="C626">
         <v>0</v>
@@ -9076,7 +9076,7 @@
         <v>350</v>
       </c>
       <c r="B627" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C627">
         <v>0</v>
@@ -9087,7 +9087,7 @@
         <v>350</v>
       </c>
       <c r="B628" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C628">
         <v>0</v>
@@ -9098,7 +9098,7 @@
         <v>350</v>
       </c>
       <c r="B629" t="s">
-        <v>352</v>
+        <v>15</v>
       </c>
       <c r="C629">
         <v>0</v>
@@ -9109,7 +9109,7 @@
         <v>350</v>
       </c>
       <c r="B630" t="s">
-        <v>24</v>
+        <v>352</v>
       </c>
       <c r="C630">
         <v>0</v>
@@ -9120,7 +9120,7 @@
         <v>350</v>
       </c>
       <c r="B631" t="s">
-        <v>88</v>
+        <v>24</v>
       </c>
       <c r="C631">
         <v>0</v>
@@ -9131,7 +9131,7 @@
         <v>350</v>
       </c>
       <c r="B632" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="C632">
         <v>0</v>
@@ -9142,7 +9142,7 @@
         <v>350</v>
       </c>
       <c r="B633" t="s">
-        <v>353</v>
+        <v>4</v>
       </c>
       <c r="C633">
         <v>0</v>
@@ -9153,7 +9153,7 @@
         <v>350</v>
       </c>
       <c r="B634" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C634">
         <v>0</v>
@@ -9164,7 +9164,7 @@
         <v>350</v>
       </c>
       <c r="B635" t="s">
-        <v>33</v>
+        <v>354</v>
       </c>
       <c r="C635">
         <v>0</v>
@@ -9175,7 +9175,7 @@
         <v>350</v>
       </c>
       <c r="B636" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C636">
         <v>0</v>
@@ -9186,7 +9186,7 @@
         <v>350</v>
       </c>
       <c r="B637" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="C637">
         <v>0</v>
@@ -9197,7 +9197,7 @@
         <v>350</v>
       </c>
       <c r="B638" t="s">
-        <v>355</v>
+        <v>69</v>
       </c>
       <c r="C638">
         <v>0</v>
@@ -9208,7 +9208,7 @@
         <v>350</v>
       </c>
       <c r="B639" t="s">
-        <v>58</v>
+        <v>355</v>
       </c>
       <c r="C639">
         <v>0</v>
@@ -9219,44 +9219,44 @@
         <v>350</v>
       </c>
       <c r="B640" t="s">
+        <v>58</v>
+      </c>
+      <c r="C640">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="641" spans="1:4">
+      <c r="A641" t="s">
+        <v>350</v>
+      </c>
+      <c r="B641" t="s">
         <v>7</v>
       </c>
-      <c r="C640">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="641" spans="1:4">
-      <c r="A641" s="2" t="s">
+      <c r="C641">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="642" spans="1:4">
+      <c r="A642" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="B641" s="2" t="s">
+      <c r="B642" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C641">
-        <v>1</v>
-      </c>
-      <c r="D641" s="2"/>
-    </row>
-    <row r="642" spans="1:4">
-      <c r="A642" t="s">
-        <v>356</v>
-      </c>
-      <c r="B642" t="s">
-        <v>5</v>
-      </c>
       <c r="C642">
         <v>1</v>
       </c>
+      <c r="D642" s="2"/>
     </row>
     <row r="643" spans="1:4">
       <c r="A643" t="s">
         <v>356</v>
       </c>
       <c r="B643" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C643">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="644" spans="1:4">
@@ -9264,10 +9264,10 @@
         <v>356</v>
       </c>
       <c r="B644" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="C644">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="645" spans="1:4">
@@ -9275,7 +9275,7 @@
         <v>356</v>
       </c>
       <c r="B645" t="s">
-        <v>337</v>
+        <v>38</v>
       </c>
       <c r="C645">
         <v>1</v>
@@ -9286,10 +9286,10 @@
         <v>356</v>
       </c>
       <c r="B646" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C646">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="647" spans="1:4">
@@ -9297,10 +9297,10 @@
         <v>356</v>
       </c>
       <c r="B647" t="s">
-        <v>36</v>
+        <v>338</v>
       </c>
       <c r="C647">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="648" spans="1:4">
@@ -9308,10 +9308,10 @@
         <v>356</v>
       </c>
       <c r="B648" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="C648">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="649" spans="1:4">
@@ -9319,7 +9319,7 @@
         <v>356</v>
       </c>
       <c r="B649" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C649">
         <v>0</v>
@@ -9330,7 +9330,7 @@
         <v>356</v>
       </c>
       <c r="B650" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C650">
         <v>0</v>
@@ -9341,7 +9341,7 @@
         <v>356</v>
       </c>
       <c r="B651" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C651">
         <v>0</v>
@@ -9352,7 +9352,7 @@
         <v>356</v>
       </c>
       <c r="B652" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C652">
         <v>0</v>
@@ -9363,7 +9363,7 @@
         <v>356</v>
       </c>
       <c r="B653" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C653">
         <v>0</v>
@@ -9374,7 +9374,7 @@
         <v>356</v>
       </c>
       <c r="B654" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C654">
         <v>0</v>
@@ -9385,7 +9385,7 @@
         <v>356</v>
       </c>
       <c r="B655" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="C655">
         <v>0</v>
@@ -9396,7 +9396,7 @@
         <v>356</v>
       </c>
       <c r="B656" t="s">
-        <v>357</v>
+        <v>20</v>
       </c>
       <c r="C656">
         <v>0</v>
@@ -9407,7 +9407,7 @@
         <v>356</v>
       </c>
       <c r="B657" t="s">
-        <v>50</v>
+        <v>357</v>
       </c>
       <c r="C657">
         <v>0</v>
@@ -9418,7 +9418,7 @@
         <v>356</v>
       </c>
       <c r="B658" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C658">
         <v>0</v>
@@ -9429,7 +9429,7 @@
         <v>356</v>
       </c>
       <c r="B659" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C659">
         <v>0</v>
@@ -9440,7 +9440,7 @@
         <v>356</v>
       </c>
       <c r="B660" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="C660">
         <v>0</v>
@@ -9451,7 +9451,7 @@
         <v>356</v>
       </c>
       <c r="B661" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C661">
         <v>0</v>
@@ -9462,7 +9462,7 @@
         <v>356</v>
       </c>
       <c r="B662" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="C662">
         <v>0</v>
@@ -9473,7 +9473,7 @@
         <v>356</v>
       </c>
       <c r="B663" t="s">
-        <v>358</v>
+        <v>45</v>
       </c>
       <c r="C663">
         <v>0</v>
@@ -9484,7 +9484,7 @@
         <v>356</v>
       </c>
       <c r="B664" t="s">
-        <v>4</v>
+        <v>358</v>
       </c>
       <c r="C664">
         <v>0</v>
@@ -9495,7 +9495,7 @@
         <v>356</v>
       </c>
       <c r="B665" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="C665">
         <v>0</v>
@@ -9506,7 +9506,7 @@
         <v>356</v>
       </c>
       <c r="B666" t="s">
-        <v>359</v>
+        <v>40</v>
       </c>
       <c r="C666">
         <v>0</v>
@@ -9517,7 +9517,7 @@
         <v>356</v>
       </c>
       <c r="B667" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C667">
         <v>0</v>
@@ -9528,41 +9528,41 @@
         <v>356</v>
       </c>
       <c r="B668" t="s">
+        <v>360</v>
+      </c>
+      <c r="C668">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="669" spans="1:4">
+      <c r="A669" t="s">
+        <v>356</v>
+      </c>
+      <c r="B669" t="s">
         <v>361</v>
       </c>
-      <c r="C668">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="669" spans="1:4">
-      <c r="A669" s="2" t="s">
+      <c r="C669">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="670" spans="1:4">
+      <c r="A670" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="B669" s="2" t="s">
+      <c r="B670" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C669">
-        <v>0</v>
-      </c>
-      <c r="D669" s="2"/>
-    </row>
-    <row r="670" spans="1:4">
-      <c r="A670" t="s">
-        <v>362</v>
-      </c>
-      <c r="B670" t="s">
-        <v>36</v>
-      </c>
       <c r="C670">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D670" s="2"/>
     </row>
     <row r="671" spans="1:4">
       <c r="A671" t="s">
         <v>362</v>
       </c>
       <c r="B671" t="s">
-        <v>363</v>
+        <v>36</v>
       </c>
       <c r="C671">
         <v>1</v>
@@ -9573,10 +9573,10 @@
         <v>362</v>
       </c>
       <c r="B672" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C672">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="673" spans="1:4">
@@ -9584,10 +9584,10 @@
         <v>362</v>
       </c>
       <c r="B673" t="s">
-        <v>338</v>
+        <v>364</v>
       </c>
       <c r="C673">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="674" spans="1:4">
@@ -9595,10 +9595,10 @@
         <v>362</v>
       </c>
       <c r="B674" t="s">
-        <v>365</v>
+        <v>338</v>
       </c>
       <c r="C674">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="675" spans="1:4">
@@ -9606,7 +9606,7 @@
         <v>362</v>
       </c>
       <c r="B675" t="s">
-        <v>355</v>
+        <v>365</v>
       </c>
       <c r="C675">
         <v>0</v>
@@ -9617,44 +9617,44 @@
         <v>362</v>
       </c>
       <c r="B676" t="s">
+        <v>355</v>
+      </c>
+      <c r="C676">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="677" spans="1:4">
+      <c r="A677" t="s">
+        <v>362</v>
+      </c>
+      <c r="B677" t="s">
         <v>366</v>
       </c>
-      <c r="C676">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="677" spans="1:4">
-      <c r="A677" s="2" t="s">
+      <c r="C677">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="678" spans="1:4">
+      <c r="A678" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="B677" s="2" t="s">
+      <c r="B678" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C677" s="2">
-        <v>0</v>
-      </c>
-      <c r="D677" s="2"/>
-    </row>
-    <row r="678" spans="1:4">
-      <c r="A678" t="s">
-        <v>367</v>
-      </c>
-      <c r="B678" t="s">
-        <v>5</v>
-      </c>
-      <c r="C678">
-        <v>1</v>
-      </c>
+      <c r="C678" s="2">
+        <v>0</v>
+      </c>
+      <c r="D678" s="2"/>
     </row>
     <row r="679" spans="1:4">
       <c r="A679" t="s">
         <v>367</v>
       </c>
       <c r="B679" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C679">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="680" spans="1:4">
@@ -9662,7 +9662,7 @@
         <v>367</v>
       </c>
       <c r="B680" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C680">
         <v>0</v>
@@ -9673,10 +9673,10 @@
         <v>367</v>
       </c>
       <c r="B681" t="s">
-        <v>368</v>
+        <v>6</v>
       </c>
       <c r="C681">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="682" spans="1:4">
@@ -9684,10 +9684,10 @@
         <v>367</v>
       </c>
       <c r="B682" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C682">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="683" spans="1:4">
@@ -9695,7 +9695,7 @@
         <v>367</v>
       </c>
       <c r="B683" t="s">
-        <v>253</v>
+        <v>369</v>
       </c>
       <c r="C683">
         <v>0</v>
@@ -9706,7 +9706,7 @@
         <v>367</v>
       </c>
       <c r="B684" t="s">
-        <v>112</v>
+        <v>253</v>
       </c>
       <c r="C684">
         <v>0</v>
@@ -9717,7 +9717,7 @@
         <v>367</v>
       </c>
       <c r="B685" t="s">
-        <v>370</v>
+        <v>112</v>
       </c>
       <c r="C685">
         <v>0</v>
@@ -9728,41 +9728,41 @@
         <v>367</v>
       </c>
       <c r="B686" t="s">
+        <v>370</v>
+      </c>
+      <c r="C686">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="687" spans="1:4">
+      <c r="A687" t="s">
+        <v>367</v>
+      </c>
+      <c r="B687" t="s">
         <v>9</v>
       </c>
-      <c r="C686">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="687" spans="1:4">
-      <c r="A687" s="2" t="s">
+      <c r="C687">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="688" spans="1:4">
+      <c r="A688" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="B687" s="2" t="s">
+      <c r="B688" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C687" s="2">
-        <v>1</v>
-      </c>
-      <c r="D687" s="2"/>
-    </row>
-    <row r="688" spans="1:4">
-      <c r="A688" t="s">
-        <v>371</v>
-      </c>
-      <c r="B688" t="s">
-        <v>36</v>
-      </c>
-      <c r="C688">
-        <v>1</v>
-      </c>
+      <c r="C688" s="2">
+        <v>1</v>
+      </c>
+      <c r="D688" s="2"/>
     </row>
     <row r="689" spans="1:4">
       <c r="A689" t="s">
         <v>371</v>
       </c>
       <c r="B689" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="C689">
         <v>1</v>
@@ -9773,10 +9773,10 @@
         <v>371</v>
       </c>
       <c r="B690" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C690">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="691" spans="1:4">
@@ -9784,10 +9784,10 @@
         <v>371</v>
       </c>
       <c r="B691" t="s">
-        <v>341</v>
+        <v>6</v>
       </c>
       <c r="C691">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="692" spans="1:4">
@@ -9795,7 +9795,7 @@
         <v>371</v>
       </c>
       <c r="B692" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C692">
         <v>1</v>
@@ -9806,7 +9806,7 @@
         <v>371</v>
       </c>
       <c r="B693" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C693">
         <v>1</v>
@@ -9817,10 +9817,10 @@
         <v>371</v>
       </c>
       <c r="B694" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C694">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="695" spans="1:4">
@@ -9828,7 +9828,7 @@
         <v>371</v>
       </c>
       <c r="B695" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C695">
         <v>0</v>
@@ -9839,7 +9839,7 @@
         <v>371</v>
       </c>
       <c r="B696" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C696">
         <v>0</v>
@@ -9850,7 +9850,7 @@
         <v>371</v>
       </c>
       <c r="B697" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C697">
         <v>0</v>
@@ -9861,23 +9861,34 @@
         <v>371</v>
       </c>
       <c r="B698" t="s">
+        <v>347</v>
+      </c>
+      <c r="C698">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="699" spans="1:4">
+      <c r="A699" t="s">
+        <v>371</v>
+      </c>
+      <c r="B699" t="s">
         <v>348</v>
       </c>
-      <c r="C698">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="699" spans="1:4">
-      <c r="A699" s="2" t="s">
+      <c r="C699">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="700" spans="1:4">
+      <c r="A700" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="B699" s="2" t="s">
+      <c r="B700" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="C699" s="2">
-        <v>0</v>
-      </c>
-      <c r="D699" s="2"/>
+      <c r="C700" s="2">
+        <v>0</v>
+      </c>
+      <c r="D700" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Atualização Mapeamento Stage LN e ODS
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Mapeamento ODS_LN.xlsx
+++ b/Documentação/Planilhas/Mapeamento ODS_LN.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1592" uniqueCount="416">
   <si>
     <t>TABELA</t>
   </si>
@@ -1328,8 +1328,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:D794" totalsRowShown="0">
-  <autoFilter ref="A1:D794">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:D795" totalsRowShown="0">
+  <autoFilter ref="A1:D795">
     <filterColumn colId="0"/>
   </autoFilter>
   <sortState ref="A2:D734">
@@ -1630,11 +1630,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D794"/>
+  <dimension ref="A1:D795"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A497" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F511" sqref="F511"/>
+      <pane ySplit="1" topLeftCell="A596" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H578" sqref="H578"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8781,12 +8781,15 @@
     </row>
     <row r="581" spans="1:4">
       <c r="A581" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="B581" t="s">
-        <v>5</v>
+        <v>388</v>
       </c>
       <c r="C581">
+        <v>0</v>
+      </c>
+      <c r="D581">
         <v>1</v>
       </c>
     </row>
@@ -8795,10 +8798,10 @@
         <v>213</v>
       </c>
       <c r="B582" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C582">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="583" spans="1:4">
@@ -8806,10 +8809,10 @@
         <v>213</v>
       </c>
       <c r="B583" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C583">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="584" spans="1:4">
@@ -8817,10 +8820,10 @@
         <v>213</v>
       </c>
       <c r="B584" t="s">
-        <v>135</v>
+        <v>25</v>
       </c>
       <c r="C584">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="585" spans="1:4">
@@ -8828,13 +8831,10 @@
         <v>213</v>
       </c>
       <c r="B585" t="s">
-        <v>62</v>
+        <v>135</v>
       </c>
       <c r="C585">
         <v>0</v>
-      </c>
-      <c r="D585">
-        <v>1</v>
       </c>
     </row>
     <row r="586" spans="1:4">
@@ -8842,7 +8842,7 @@
         <v>213</v>
       </c>
       <c r="B586" t="s">
-        <v>140</v>
+        <v>62</v>
       </c>
       <c r="C586">
         <v>0</v>
@@ -8856,7 +8856,7 @@
         <v>213</v>
       </c>
       <c r="B587" t="s">
-        <v>214</v>
+        <v>140</v>
       </c>
       <c r="C587">
         <v>0</v>
@@ -8870,7 +8870,7 @@
         <v>213</v>
       </c>
       <c r="B588" t="s">
-        <v>161</v>
+        <v>214</v>
       </c>
       <c r="C588">
         <v>0</v>
@@ -8884,10 +8884,13 @@
         <v>213</v>
       </c>
       <c r="B589" t="s">
-        <v>215</v>
+        <v>161</v>
       </c>
       <c r="C589">
         <v>0</v>
+      </c>
+      <c r="D589">
+        <v>1</v>
       </c>
     </row>
     <row r="590" spans="1:4">
@@ -8895,13 +8898,10 @@
         <v>213</v>
       </c>
       <c r="B590" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C590">
         <v>0</v>
-      </c>
-      <c r="D590">
-        <v>1</v>
       </c>
     </row>
     <row r="591" spans="1:4">
@@ -8909,10 +8909,13 @@
         <v>213</v>
       </c>
       <c r="B591" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C591">
         <v>0</v>
+      </c>
+      <c r="D591">
+        <v>1</v>
       </c>
     </row>
     <row r="592" spans="1:4">
@@ -8920,13 +8923,10 @@
         <v>213</v>
       </c>
       <c r="B592" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C592">
         <v>0</v>
-      </c>
-      <c r="D592">
-        <v>1</v>
       </c>
     </row>
     <row r="593" spans="1:4">
@@ -8934,7 +8934,7 @@
         <v>213</v>
       </c>
       <c r="B593" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C593">
         <v>0</v>
@@ -8948,7 +8948,7 @@
         <v>213</v>
       </c>
       <c r="B594" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C594">
         <v>0</v>
@@ -8962,7 +8962,7 @@
         <v>213</v>
       </c>
       <c r="B595" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C595">
         <v>0</v>
@@ -8976,7 +8976,7 @@
         <v>213</v>
       </c>
       <c r="B596" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C596">
         <v>0</v>
@@ -8990,7 +8990,7 @@
         <v>213</v>
       </c>
       <c r="B597" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C597">
         <v>0</v>
@@ -9004,7 +9004,7 @@
         <v>213</v>
       </c>
       <c r="B598" t="s">
-        <v>388</v>
+        <v>223</v>
       </c>
       <c r="C598">
         <v>0</v>
@@ -9018,7 +9018,7 @@
         <v>213</v>
       </c>
       <c r="B599" t="s">
-        <v>224</v>
+        <v>388</v>
       </c>
       <c r="C599">
         <v>0</v>
@@ -9032,10 +9032,13 @@
         <v>213</v>
       </c>
       <c r="B600" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C600">
         <v>0</v>
+      </c>
+      <c r="D600">
+        <v>1</v>
       </c>
     </row>
     <row r="601" spans="1:4">
@@ -9043,13 +9046,10 @@
         <v>213</v>
       </c>
       <c r="B601" t="s">
-        <v>84</v>
+        <v>226</v>
       </c>
       <c r="C601">
         <v>0</v>
-      </c>
-      <c r="D601">
-        <v>1</v>
       </c>
     </row>
     <row r="602" spans="1:4">
@@ -9057,7 +9057,7 @@
         <v>213</v>
       </c>
       <c r="B602" t="s">
-        <v>227</v>
+        <v>84</v>
       </c>
       <c r="C602">
         <v>0</v>
@@ -9071,7 +9071,7 @@
         <v>213</v>
       </c>
       <c r="B603" t="s">
-        <v>199</v>
+        <v>227</v>
       </c>
       <c r="C603">
         <v>0</v>
@@ -9085,10 +9085,13 @@
         <v>213</v>
       </c>
       <c r="B604" t="s">
-        <v>228</v>
+        <v>199</v>
       </c>
       <c r="C604">
         <v>0</v>
+      </c>
+      <c r="D604">
+        <v>1</v>
       </c>
     </row>
     <row r="605" spans="1:4">
@@ -9096,7 +9099,7 @@
         <v>213</v>
       </c>
       <c r="B605" t="s">
-        <v>33</v>
+        <v>228</v>
       </c>
       <c r="C605">
         <v>0</v>
@@ -9107,13 +9110,10 @@
         <v>213</v>
       </c>
       <c r="B606" t="s">
-        <v>229</v>
+        <v>33</v>
       </c>
       <c r="C606">
         <v>0</v>
-      </c>
-      <c r="D606">
-        <v>1</v>
       </c>
     </row>
     <row r="607" spans="1:4">
@@ -9121,7 +9121,7 @@
         <v>213</v>
       </c>
       <c r="B607" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C607">
         <v>0</v>
@@ -9135,10 +9135,13 @@
         <v>213</v>
       </c>
       <c r="B608" t="s">
-        <v>23</v>
+        <v>230</v>
       </c>
       <c r="C608">
         <v>0</v>
+      </c>
+      <c r="D608">
+        <v>1</v>
       </c>
     </row>
     <row r="609" spans="1:4">
@@ -9146,7 +9149,7 @@
         <v>213</v>
       </c>
       <c r="B609" t="s">
-        <v>231</v>
+        <v>23</v>
       </c>
       <c r="C609">
         <v>0</v>
@@ -9157,23 +9160,23 @@
         <v>213</v>
       </c>
       <c r="B610" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C610">
         <v>0</v>
-      </c>
-      <c r="D610">
-        <v>1</v>
       </c>
     </row>
     <row r="611" spans="1:4">
       <c r="A611" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="B611" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="C611">
+        <v>0</v>
+      </c>
+      <c r="D611">
         <v>1</v>
       </c>
     </row>
@@ -9182,7 +9185,7 @@
         <v>233</v>
       </c>
       <c r="B612" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="C612">
         <v>1</v>
@@ -9193,10 +9196,10 @@
         <v>233</v>
       </c>
       <c r="B613" t="s">
-        <v>178</v>
+        <v>25</v>
       </c>
       <c r="C613">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="614" spans="1:4">
@@ -9204,10 +9207,10 @@
         <v>233</v>
       </c>
       <c r="B614" t="s">
-        <v>79</v>
+        <v>178</v>
       </c>
       <c r="C614">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="615" spans="1:4">
@@ -9215,10 +9218,10 @@
         <v>233</v>
       </c>
       <c r="B615" t="s">
-        <v>234</v>
+        <v>79</v>
       </c>
       <c r="C615">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="616" spans="1:4">
@@ -9226,13 +9229,10 @@
         <v>233</v>
       </c>
       <c r="B616" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C616">
         <v>0</v>
-      </c>
-      <c r="D616">
-        <v>1</v>
       </c>
     </row>
     <row r="617" spans="1:4">
@@ -9240,7 +9240,7 @@
         <v>233</v>
       </c>
       <c r="B617" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C617">
         <v>0</v>
@@ -9254,7 +9254,7 @@
         <v>233</v>
       </c>
       <c r="B618" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C618">
         <v>0</v>
@@ -9268,7 +9268,7 @@
         <v>233</v>
       </c>
       <c r="B619" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C619">
         <v>0</v>
@@ -9282,7 +9282,7 @@
         <v>233</v>
       </c>
       <c r="B620" t="s">
-        <v>119</v>
+        <v>238</v>
       </c>
       <c r="C620">
         <v>0</v>
@@ -9296,7 +9296,7 @@
         <v>233</v>
       </c>
       <c r="B621" t="s">
-        <v>239</v>
+        <v>119</v>
       </c>
       <c r="C621">
         <v>0</v>
@@ -9310,7 +9310,7 @@
         <v>233</v>
       </c>
       <c r="B622" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C622">
         <v>0</v>
@@ -9324,7 +9324,7 @@
         <v>233</v>
       </c>
       <c r="B623" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C623">
         <v>0</v>
@@ -9338,7 +9338,7 @@
         <v>233</v>
       </c>
       <c r="B624" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C624">
         <v>0</v>
@@ -9352,7 +9352,7 @@
         <v>233</v>
       </c>
       <c r="B625" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C625">
         <v>0</v>
@@ -9366,7 +9366,7 @@
         <v>233</v>
       </c>
       <c r="B626" t="s">
-        <v>388</v>
+        <v>243</v>
       </c>
       <c r="C626">
         <v>0</v>
@@ -9380,7 +9380,7 @@
         <v>233</v>
       </c>
       <c r="B627" t="s">
-        <v>244</v>
+        <v>388</v>
       </c>
       <c r="C627">
         <v>0</v>
@@ -9394,7 +9394,7 @@
         <v>233</v>
       </c>
       <c r="B628" t="s">
-        <v>84</v>
+        <v>244</v>
       </c>
       <c r="C628">
         <v>0</v>
@@ -9408,7 +9408,7 @@
         <v>233</v>
       </c>
       <c r="B629" t="s">
-        <v>227</v>
+        <v>84</v>
       </c>
       <c r="C629">
         <v>0</v>
@@ -9422,7 +9422,7 @@
         <v>233</v>
       </c>
       <c r="B630" t="s">
-        <v>199</v>
+        <v>227</v>
       </c>
       <c r="C630">
         <v>0</v>
@@ -9436,10 +9436,13 @@
         <v>233</v>
       </c>
       <c r="B631" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="C631">
         <v>0</v>
+      </c>
+      <c r="D631">
+        <v>1</v>
       </c>
     </row>
     <row r="632" spans="1:4">
@@ -9447,7 +9450,7 @@
         <v>233</v>
       </c>
       <c r="B632" t="s">
-        <v>62</v>
+        <v>191</v>
       </c>
       <c r="C632">
         <v>0</v>
@@ -9455,16 +9458,13 @@
     </row>
     <row r="633" spans="1:4">
       <c r="A633" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="B633" t="s">
-        <v>388</v>
+        <v>62</v>
       </c>
       <c r="C633">
         <v>0</v>
-      </c>
-      <c r="D633">
-        <v>1</v>
       </c>
     </row>
     <row r="634" spans="1:4">
@@ -9472,9 +9472,12 @@
         <v>245</v>
       </c>
       <c r="B634" t="s">
-        <v>5</v>
+        <v>388</v>
       </c>
       <c r="C634">
+        <v>0</v>
+      </c>
+      <c r="D634">
         <v>1</v>
       </c>
     </row>
@@ -9483,7 +9486,7 @@
         <v>245</v>
       </c>
       <c r="B635" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="C635">
         <v>1</v>
@@ -9494,10 +9497,10 @@
         <v>245</v>
       </c>
       <c r="B636" t="s">
-        <v>246</v>
+        <v>70</v>
       </c>
       <c r="C636">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="637" spans="1:4">
@@ -9505,7 +9508,7 @@
         <v>245</v>
       </c>
       <c r="B637" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C637">
         <v>0</v>
@@ -9516,7 +9519,7 @@
         <v>245</v>
       </c>
       <c r="B638" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C638">
         <v>0</v>
@@ -9527,7 +9530,7 @@
         <v>245</v>
       </c>
       <c r="B639" t="s">
-        <v>111</v>
+        <v>248</v>
       </c>
       <c r="C639">
         <v>0</v>
@@ -9538,7 +9541,7 @@
         <v>245</v>
       </c>
       <c r="B640" t="s">
-        <v>249</v>
+        <v>111</v>
       </c>
       <c r="C640">
         <v>0</v>
@@ -9549,10 +9552,10 @@
         <v>245</v>
       </c>
       <c r="B641" t="s">
-        <v>69</v>
+        <v>249</v>
       </c>
       <c r="C641">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="642" spans="1:4">
@@ -9560,10 +9563,10 @@
         <v>245</v>
       </c>
       <c r="B642" t="s">
-        <v>115</v>
+        <v>69</v>
       </c>
       <c r="C642">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="643" spans="1:4">
@@ -9571,7 +9574,7 @@
         <v>245</v>
       </c>
       <c r="B643" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C643">
         <v>0</v>
@@ -9582,7 +9585,7 @@
         <v>245</v>
       </c>
       <c r="B644" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="C644">
         <v>0</v>
@@ -9593,7 +9596,7 @@
         <v>245</v>
       </c>
       <c r="B645" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C645">
         <v>0</v>
@@ -9604,7 +9607,7 @@
         <v>245</v>
       </c>
       <c r="B646" t="s">
-        <v>250</v>
+        <v>63</v>
       </c>
       <c r="C646">
         <v>0</v>
@@ -9615,13 +9618,10 @@
         <v>245</v>
       </c>
       <c r="B647" t="s">
-        <v>221</v>
+        <v>250</v>
       </c>
       <c r="C647">
         <v>0</v>
-      </c>
-      <c r="D647">
-        <v>1</v>
       </c>
     </row>
     <row r="648" spans="1:4">
@@ -9629,7 +9629,7 @@
         <v>245</v>
       </c>
       <c r="B648" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C648">
         <v>0</v>
@@ -9643,7 +9643,7 @@
         <v>245</v>
       </c>
       <c r="B649" t="s">
-        <v>251</v>
+        <v>222</v>
       </c>
       <c r="C649">
         <v>0</v>
@@ -9657,7 +9657,7 @@
         <v>245</v>
       </c>
       <c r="B650" t="s">
-        <v>85</v>
+        <v>251</v>
       </c>
       <c r="C650">
         <v>0</v>
@@ -9671,10 +9671,13 @@
         <v>245</v>
       </c>
       <c r="B651" t="s">
-        <v>252</v>
+        <v>85</v>
       </c>
       <c r="C651">
         <v>0</v>
+      </c>
+      <c r="D651">
+        <v>1</v>
       </c>
     </row>
     <row r="652" spans="1:4">
@@ -9682,7 +9685,7 @@
         <v>245</v>
       </c>
       <c r="B652" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C652">
         <v>0</v>
@@ -9693,7 +9696,7 @@
         <v>245</v>
       </c>
       <c r="B653" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C653">
         <v>0</v>
@@ -9704,13 +9707,10 @@
         <v>245</v>
       </c>
       <c r="B654" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C654">
         <v>0</v>
-      </c>
-      <c r="D654">
-        <v>1</v>
       </c>
     </row>
     <row r="655" spans="1:4">
@@ -9718,7 +9718,7 @@
         <v>245</v>
       </c>
       <c r="B655" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C655">
         <v>0</v>
@@ -9732,10 +9732,13 @@
         <v>245</v>
       </c>
       <c r="B656" t="s">
-        <v>108</v>
+        <v>256</v>
       </c>
       <c r="C656">
         <v>0</v>
+      </c>
+      <c r="D656">
+        <v>1</v>
       </c>
     </row>
     <row r="657" spans="1:4">
@@ -9743,7 +9746,7 @@
         <v>245</v>
       </c>
       <c r="B657" t="s">
-        <v>257</v>
+        <v>108</v>
       </c>
       <c r="C657">
         <v>0</v>
@@ -9754,7 +9757,7 @@
         <v>245</v>
       </c>
       <c r="B658" t="s">
-        <v>277</v>
+        <v>257</v>
       </c>
       <c r="C658">
         <v>0</v>
@@ -9765,7 +9768,7 @@
         <v>245</v>
       </c>
       <c r="B659" t="s">
-        <v>258</v>
+        <v>277</v>
       </c>
       <c r="C659">
         <v>0</v>
@@ -9776,41 +9779,41 @@
         <v>245</v>
       </c>
       <c r="B660" t="s">
+        <v>258</v>
+      </c>
+      <c r="C660">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="661" spans="1:4">
+      <c r="A661" t="s">
+        <v>245</v>
+      </c>
+      <c r="B661" t="s">
         <v>259</v>
       </c>
-      <c r="C660">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="661" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A661" s="3" t="s">
+      <c r="C661">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="662" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A662" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="B661" s="3" t="s">
+      <c r="B662" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C661" s="3">
-        <v>0</v>
-      </c>
-      <c r="D661" s="3"/>
-    </row>
-    <row r="662" spans="1:4" ht="15.75" thickTop="1">
-      <c r="A662" t="s">
-        <v>245</v>
-      </c>
-      <c r="B662" t="s">
-        <v>260</v>
-      </c>
-      <c r="C662">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="663" spans="1:4">
+      <c r="C662" s="3">
+        <v>0</v>
+      </c>
+      <c r="D662" s="3"/>
+    </row>
+    <row r="663" spans="1:4" ht="15.75" thickTop="1">
       <c r="A663" t="s">
         <v>245</v>
       </c>
       <c r="B663" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C663">
         <v>0</v>
@@ -9821,7 +9824,7 @@
         <v>245</v>
       </c>
       <c r="B664" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C664">
         <v>0</v>
@@ -9832,7 +9835,7 @@
         <v>245</v>
       </c>
       <c r="B665" t="s">
-        <v>125</v>
+        <v>262</v>
       </c>
       <c r="C665">
         <v>0</v>
@@ -9843,7 +9846,7 @@
         <v>245</v>
       </c>
       <c r="B666" t="s">
-        <v>263</v>
+        <v>125</v>
       </c>
       <c r="C666">
         <v>0</v>
@@ -9854,7 +9857,7 @@
         <v>245</v>
       </c>
       <c r="B667" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C667">
         <v>0</v>
@@ -9865,13 +9868,10 @@
         <v>245</v>
       </c>
       <c r="B668" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C668">
         <v>0</v>
-      </c>
-      <c r="D668">
-        <v>1</v>
       </c>
     </row>
     <row r="669" spans="1:4">
@@ -9879,7 +9879,7 @@
         <v>245</v>
       </c>
       <c r="B669" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C669">
         <v>0</v>
@@ -9893,10 +9893,13 @@
         <v>245</v>
       </c>
       <c r="B670" t="s">
-        <v>75</v>
+        <v>266</v>
       </c>
       <c r="C670">
         <v>0</v>
+      </c>
+      <c r="D670">
+        <v>1</v>
       </c>
     </row>
     <row r="671" spans="1:4">
@@ -9904,7 +9907,7 @@
         <v>245</v>
       </c>
       <c r="B671" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C671">
         <v>0</v>
@@ -9915,7 +9918,7 @@
         <v>245</v>
       </c>
       <c r="B672" t="s">
-        <v>267</v>
+        <v>76</v>
       </c>
       <c r="C672">
         <v>0</v>
@@ -9926,13 +9929,10 @@
         <v>245</v>
       </c>
       <c r="B673" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C673">
         <v>0</v>
-      </c>
-      <c r="D673">
-        <v>1</v>
       </c>
     </row>
     <row r="674" spans="1:4">
@@ -9940,10 +9940,13 @@
         <v>245</v>
       </c>
       <c r="B674" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C674">
         <v>0</v>
+      </c>
+      <c r="D674">
+        <v>1</v>
       </c>
     </row>
     <row r="675" spans="1:4">
@@ -9951,7 +9954,7 @@
         <v>245</v>
       </c>
       <c r="B675" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C675">
         <v>0</v>
@@ -9962,7 +9965,7 @@
         <v>245</v>
       </c>
       <c r="B676" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C676">
         <v>0</v>
@@ -9973,7 +9976,7 @@
         <v>245</v>
       </c>
       <c r="B677" t="s">
-        <v>123</v>
+        <v>271</v>
       </c>
       <c r="C677">
         <v>0</v>
@@ -9984,7 +9987,7 @@
         <v>245</v>
       </c>
       <c r="B678" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C678">
         <v>0</v>
@@ -9995,7 +9998,7 @@
         <v>245</v>
       </c>
       <c r="B679" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="C679">
         <v>0</v>
@@ -10006,7 +10009,7 @@
         <v>245</v>
       </c>
       <c r="B680" t="s">
-        <v>272</v>
+        <v>118</v>
       </c>
       <c r="C680">
         <v>0</v>
@@ -10017,13 +10020,10 @@
         <v>245</v>
       </c>
       <c r="B681" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C681">
         <v>0</v>
-      </c>
-      <c r="D681">
-        <v>1</v>
       </c>
     </row>
     <row r="682" spans="1:4">
@@ -10031,7 +10031,7 @@
         <v>245</v>
       </c>
       <c r="B682" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C682">
         <v>0</v>
@@ -10045,10 +10045,13 @@
         <v>245</v>
       </c>
       <c r="B683" t="s">
-        <v>33</v>
+        <v>274</v>
       </c>
       <c r="C683">
         <v>0</v>
+      </c>
+      <c r="D683">
+        <v>1</v>
       </c>
     </row>
     <row r="684" spans="1:4">
@@ -10056,7 +10059,7 @@
         <v>245</v>
       </c>
       <c r="B684" t="s">
-        <v>333</v>
+        <v>33</v>
       </c>
       <c r="C684">
         <v>0</v>
@@ -10067,7 +10070,7 @@
         <v>245</v>
       </c>
       <c r="B685" t="s">
-        <v>415</v>
+        <v>333</v>
       </c>
       <c r="C685">
         <v>0</v>
@@ -10075,13 +10078,13 @@
     </row>
     <row r="686" spans="1:4">
       <c r="A686" t="s">
-        <v>275</v>
+        <v>245</v>
       </c>
       <c r="B686" t="s">
-        <v>5</v>
+        <v>415</v>
       </c>
       <c r="C686">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="687" spans="1:4">
@@ -10089,7 +10092,7 @@
         <v>275</v>
       </c>
       <c r="B687" t="s">
-        <v>68</v>
+        <v>5</v>
       </c>
       <c r="C687">
         <v>1</v>
@@ -10100,10 +10103,10 @@
         <v>275</v>
       </c>
       <c r="B688" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C688">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="689" spans="1:3">
@@ -10111,7 +10114,7 @@
         <v>275</v>
       </c>
       <c r="B689" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C689">
         <v>0</v>
@@ -10122,7 +10125,7 @@
         <v>275</v>
       </c>
       <c r="B690" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C690">
         <v>0</v>
@@ -10133,7 +10136,7 @@
         <v>275</v>
       </c>
       <c r="B691" t="s">
-        <v>276</v>
+        <v>65</v>
       </c>
       <c r="C691">
         <v>0</v>
@@ -10144,7 +10147,7 @@
         <v>275</v>
       </c>
       <c r="B692" t="s">
-        <v>108</v>
+        <v>276</v>
       </c>
       <c r="C692">
         <v>0</v>
@@ -10155,7 +10158,7 @@
         <v>275</v>
       </c>
       <c r="B693" t="s">
-        <v>257</v>
+        <v>108</v>
       </c>
       <c r="C693">
         <v>0</v>
@@ -10166,7 +10169,7 @@
         <v>275</v>
       </c>
       <c r="B694" t="s">
-        <v>277</v>
+        <v>257</v>
       </c>
       <c r="C694">
         <v>0</v>
@@ -10177,7 +10180,7 @@
         <v>275</v>
       </c>
       <c r="B695" t="s">
-        <v>258</v>
+        <v>277</v>
       </c>
       <c r="C695">
         <v>0</v>
@@ -10188,7 +10191,7 @@
         <v>275</v>
       </c>
       <c r="B696" t="s">
-        <v>278</v>
+        <v>258</v>
       </c>
       <c r="C696">
         <v>0</v>
@@ -10199,7 +10202,7 @@
         <v>275</v>
       </c>
       <c r="B697" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C697">
         <v>0</v>
@@ -10210,7 +10213,7 @@
         <v>275</v>
       </c>
       <c r="B698" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C698">
         <v>0</v>
@@ -10221,7 +10224,7 @@
         <v>275</v>
       </c>
       <c r="B699" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C699">
         <v>0</v>
@@ -10232,7 +10235,7 @@
         <v>275</v>
       </c>
       <c r="B700" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C700">
         <v>0</v>
@@ -10243,7 +10246,7 @@
         <v>275</v>
       </c>
       <c r="B701" t="s">
-        <v>66</v>
+        <v>282</v>
       </c>
       <c r="C701">
         <v>0</v>
@@ -10254,7 +10257,7 @@
         <v>275</v>
       </c>
       <c r="B702" t="s">
-        <v>109</v>
+        <v>66</v>
       </c>
       <c r="C702">
         <v>0</v>
@@ -10265,7 +10268,7 @@
         <v>275</v>
       </c>
       <c r="B703" t="s">
-        <v>260</v>
+        <v>109</v>
       </c>
       <c r="C703">
         <v>0</v>
@@ -10276,7 +10279,7 @@
         <v>275</v>
       </c>
       <c r="B704" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C704">
         <v>0</v>
@@ -10287,7 +10290,7 @@
         <v>275</v>
       </c>
       <c r="B705" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C705">
         <v>0</v>
@@ -10298,7 +10301,7 @@
         <v>275</v>
       </c>
       <c r="B706" t="s">
-        <v>283</v>
+        <v>262</v>
       </c>
       <c r="C706">
         <v>0</v>
@@ -10309,7 +10312,7 @@
         <v>275</v>
       </c>
       <c r="B707" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C707">
         <v>0</v>
@@ -10320,7 +10323,7 @@
         <v>275</v>
       </c>
       <c r="B708" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C708">
         <v>0</v>
@@ -10331,7 +10334,7 @@
         <v>275</v>
       </c>
       <c r="B709" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C709">
         <v>0</v>
@@ -10342,7 +10345,7 @@
         <v>275</v>
       </c>
       <c r="B710" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C710">
         <v>0</v>
@@ -10353,7 +10356,7 @@
         <v>275</v>
       </c>
       <c r="B711" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C711">
         <v>0</v>
@@ -10364,13 +10367,10 @@
         <v>275</v>
       </c>
       <c r="B712" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C712">
         <v>0</v>
-      </c>
-      <c r="D712">
-        <v>1</v>
       </c>
     </row>
     <row r="713" spans="1:4">
@@ -10378,7 +10378,7 @@
         <v>275</v>
       </c>
       <c r="B713" t="s">
-        <v>388</v>
+        <v>289</v>
       </c>
       <c r="C713">
         <v>0</v>
@@ -10392,24 +10392,24 @@
         <v>275</v>
       </c>
       <c r="B714" t="s">
-        <v>125</v>
+        <v>388</v>
       </c>
       <c r="C714">
         <v>0</v>
+      </c>
+      <c r="D714">
+        <v>1</v>
       </c>
     </row>
     <row r="715" spans="1:4">
       <c r="A715" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="B715" t="s">
-        <v>388</v>
+        <v>125</v>
       </c>
       <c r="C715">
         <v>0</v>
-      </c>
-      <c r="D715">
-        <v>1</v>
       </c>
     </row>
     <row r="716" spans="1:4">
@@ -10417,9 +10417,12 @@
         <v>290</v>
       </c>
       <c r="B716" t="s">
-        <v>5</v>
+        <v>388</v>
       </c>
       <c r="C716">
+        <v>0</v>
+      </c>
+      <c r="D716">
         <v>1</v>
       </c>
     </row>
@@ -10428,10 +10431,10 @@
         <v>290</v>
       </c>
       <c r="B717" t="s">
-        <v>111</v>
+        <v>5</v>
       </c>
       <c r="C717">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="718" spans="1:4">
@@ -10439,10 +10442,10 @@
         <v>290</v>
       </c>
       <c r="B718" t="s">
-        <v>70</v>
+        <v>111</v>
       </c>
       <c r="C718">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="719" spans="1:4">
@@ -10450,10 +10453,10 @@
         <v>290</v>
       </c>
       <c r="B719" t="s">
-        <v>247</v>
+        <v>70</v>
       </c>
       <c r="C719">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="720" spans="1:4">
@@ -10461,13 +10464,10 @@
         <v>290</v>
       </c>
       <c r="B720" t="s">
-        <v>119</v>
+        <v>247</v>
       </c>
       <c r="C720">
         <v>0</v>
-      </c>
-      <c r="D720">
-        <v>1</v>
       </c>
     </row>
     <row r="721" spans="1:4">
@@ -10475,7 +10475,7 @@
         <v>290</v>
       </c>
       <c r="B721" t="s">
-        <v>221</v>
+        <v>119</v>
       </c>
       <c r="C721">
         <v>0</v>
@@ -10489,10 +10489,13 @@
         <v>290</v>
       </c>
       <c r="B722" t="s">
-        <v>252</v>
+        <v>221</v>
       </c>
       <c r="C722">
         <v>0</v>
+      </c>
+      <c r="D722">
+        <v>1</v>
       </c>
     </row>
     <row r="723" spans="1:4">
@@ -10500,10 +10503,10 @@
         <v>290</v>
       </c>
       <c r="B723" t="s">
-        <v>79</v>
+        <v>252</v>
       </c>
       <c r="C723">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="724" spans="1:4">
@@ -10511,12 +10514,9 @@
         <v>290</v>
       </c>
       <c r="B724" t="s">
-        <v>291</v>
+        <v>79</v>
       </c>
       <c r="C724">
-        <v>0</v>
-      </c>
-      <c r="D724">
         <v>1</v>
       </c>
     </row>
@@ -10525,7 +10525,7 @@
         <v>290</v>
       </c>
       <c r="B725" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C725">
         <v>0</v>
@@ -10539,7 +10539,7 @@
         <v>290</v>
       </c>
       <c r="B726" t="s">
-        <v>105</v>
+        <v>292</v>
       </c>
       <c r="C726">
         <v>0</v>
@@ -10553,7 +10553,7 @@
         <v>290</v>
       </c>
       <c r="B727" t="s">
-        <v>251</v>
+        <v>105</v>
       </c>
       <c r="C727">
         <v>0</v>
@@ -10567,7 +10567,7 @@
         <v>290</v>
       </c>
       <c r="B728" t="s">
-        <v>85</v>
+        <v>251</v>
       </c>
       <c r="C728">
         <v>0</v>
@@ -10581,10 +10581,13 @@
         <v>290</v>
       </c>
       <c r="B729" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="C729">
         <v>0</v>
+      </c>
+      <c r="D729">
+        <v>1</v>
       </c>
     </row>
     <row r="730" spans="1:4">
@@ -10592,7 +10595,7 @@
         <v>290</v>
       </c>
       <c r="B730" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C730">
         <v>0</v>
@@ -10603,7 +10606,7 @@
         <v>290</v>
       </c>
       <c r="B731" t="s">
-        <v>293</v>
+        <v>125</v>
       </c>
       <c r="C731">
         <v>0</v>
@@ -10614,7 +10617,7 @@
         <v>290</v>
       </c>
       <c r="B732" t="s">
-        <v>53</v>
+        <v>293</v>
       </c>
       <c r="C732">
         <v>0</v>
@@ -10625,7 +10628,7 @@
         <v>290</v>
       </c>
       <c r="B733" t="s">
-        <v>294</v>
+        <v>53</v>
       </c>
       <c r="C733">
         <v>0</v>
@@ -10636,7 +10639,7 @@
         <v>290</v>
       </c>
       <c r="B734" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C734">
         <v>0</v>
@@ -10647,7 +10650,7 @@
         <v>290</v>
       </c>
       <c r="B735" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C735">
         <v>0</v>
@@ -10658,13 +10661,10 @@
         <v>290</v>
       </c>
       <c r="B736" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C736">
         <v>0</v>
-      </c>
-      <c r="D736">
-        <v>1</v>
       </c>
     </row>
     <row r="737" spans="1:4">
@@ -10672,7 +10672,7 @@
         <v>290</v>
       </c>
       <c r="B737" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C737">
         <v>0</v>
@@ -10686,7 +10686,7 @@
         <v>290</v>
       </c>
       <c r="B738" t="s">
-        <v>88</v>
+        <v>298</v>
       </c>
       <c r="C738">
         <v>0</v>
@@ -10700,7 +10700,7 @@
         <v>290</v>
       </c>
       <c r="B739" t="s">
-        <v>299</v>
+        <v>88</v>
       </c>
       <c r="C739">
         <v>0</v>
@@ -10714,10 +10714,13 @@
         <v>290</v>
       </c>
       <c r="B740" t="s">
-        <v>6</v>
+        <v>299</v>
       </c>
       <c r="C740">
         <v>0</v>
+      </c>
+      <c r="D740">
+        <v>1</v>
       </c>
     </row>
     <row r="741" spans="1:4">
@@ -10725,7 +10728,7 @@
         <v>290</v>
       </c>
       <c r="B741" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="C741">
         <v>0</v>
@@ -10736,7 +10739,7 @@
         <v>290</v>
       </c>
       <c r="B742" t="s">
-        <v>300</v>
+        <v>33</v>
       </c>
       <c r="C742">
         <v>0</v>
@@ -10747,7 +10750,7 @@
         <v>290</v>
       </c>
       <c r="B743" t="s">
-        <v>68</v>
+        <v>300</v>
       </c>
       <c r="C743">
         <v>0</v>
@@ -10758,10 +10761,10 @@
         <v>290</v>
       </c>
       <c r="B744" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C744">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="745" spans="1:4">
@@ -10769,10 +10772,10 @@
         <v>290</v>
       </c>
       <c r="B745" t="s">
-        <v>301</v>
+        <v>69</v>
       </c>
       <c r="C745">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="746" spans="1:4">
@@ -10780,7 +10783,7 @@
         <v>290</v>
       </c>
       <c r="B746" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C746">
         <v>0</v>
@@ -10791,7 +10794,7 @@
         <v>290</v>
       </c>
       <c r="B747" t="s">
-        <v>253</v>
+        <v>302</v>
       </c>
       <c r="C747">
         <v>0</v>
@@ -10802,13 +10805,10 @@
         <v>290</v>
       </c>
       <c r="B748" t="s">
-        <v>77</v>
+        <v>253</v>
       </c>
       <c r="C748">
         <v>0</v>
-      </c>
-      <c r="D748">
-        <v>1</v>
       </c>
     </row>
     <row r="749" spans="1:4">
@@ -10816,10 +10816,13 @@
         <v>290</v>
       </c>
       <c r="B749" t="s">
-        <v>328</v>
+        <v>77</v>
       </c>
       <c r="C749">
         <v>0</v>
+      </c>
+      <c r="D749">
+        <v>1</v>
       </c>
     </row>
     <row r="750" spans="1:4">
@@ -10827,10 +10830,10 @@
         <v>290</v>
       </c>
       <c r="B750" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C750">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="751" spans="1:4">
@@ -10838,24 +10841,21 @@
         <v>290</v>
       </c>
       <c r="B751" t="s">
-        <v>415</v>
+        <v>330</v>
       </c>
       <c r="C751">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="752" spans="1:4">
       <c r="A752" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
       <c r="B752" t="s">
-        <v>388</v>
+        <v>415</v>
       </c>
       <c r="C752">
         <v>0</v>
-      </c>
-      <c r="D752">
-        <v>1</v>
       </c>
     </row>
     <row r="753" spans="1:4">
@@ -10863,9 +10863,12 @@
         <v>303</v>
       </c>
       <c r="B753" t="s">
-        <v>5</v>
+        <v>388</v>
       </c>
       <c r="C753">
+        <v>0</v>
+      </c>
+      <c r="D753">
         <v>1</v>
       </c>
     </row>
@@ -10874,7 +10877,7 @@
         <v>303</v>
       </c>
       <c r="B754" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="C754">
         <v>1</v>
@@ -10885,10 +10888,10 @@
         <v>303</v>
       </c>
       <c r="B755" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C755">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="756" spans="1:4">
@@ -10896,10 +10899,10 @@
         <v>303</v>
       </c>
       <c r="B756" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C756">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="757" spans="1:4">
@@ -10907,7 +10910,7 @@
         <v>303</v>
       </c>
       <c r="B757" t="s">
-        <v>304</v>
+        <v>69</v>
       </c>
       <c r="C757">
         <v>1</v>
@@ -10918,7 +10921,7 @@
         <v>303</v>
       </c>
       <c r="B758" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C758">
         <v>1</v>
@@ -10929,10 +10932,10 @@
         <v>303</v>
       </c>
       <c r="B759" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C759">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="760" spans="1:4">
@@ -10940,7 +10943,7 @@
         <v>303</v>
       </c>
       <c r="B760" t="s">
-        <v>49</v>
+        <v>306</v>
       </c>
       <c r="C760">
         <v>0</v>
@@ -10951,7 +10954,7 @@
         <v>303</v>
       </c>
       <c r="B761" t="s">
-        <v>307</v>
+        <v>49</v>
       </c>
       <c r="C761">
         <v>0</v>
@@ -10962,13 +10965,10 @@
         <v>303</v>
       </c>
       <c r="B762" t="s">
-        <v>54</v>
+        <v>307</v>
       </c>
       <c r="C762">
         <v>0</v>
-      </c>
-      <c r="D762">
-        <v>1</v>
       </c>
     </row>
     <row r="763" spans="1:4">
@@ -10976,7 +10976,7 @@
         <v>303</v>
       </c>
       <c r="B763" t="s">
-        <v>308</v>
+        <v>54</v>
       </c>
       <c r="C763">
         <v>0</v>
@@ -10990,10 +10990,13 @@
         <v>303</v>
       </c>
       <c r="B764" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C764">
         <v>0</v>
+      </c>
+      <c r="D764">
+        <v>1</v>
       </c>
     </row>
     <row r="765" spans="1:4">
@@ -11001,13 +11004,10 @@
         <v>303</v>
       </c>
       <c r="B765" t="s">
-        <v>217</v>
+        <v>309</v>
       </c>
       <c r="C765">
         <v>0</v>
-      </c>
-      <c r="D765">
-        <v>1</v>
       </c>
     </row>
     <row r="766" spans="1:4">
@@ -11015,10 +11015,13 @@
         <v>303</v>
       </c>
       <c r="B766" t="s">
-        <v>111</v>
+        <v>217</v>
       </c>
       <c r="C766">
         <v>0</v>
+      </c>
+      <c r="D766">
+        <v>1</v>
       </c>
     </row>
     <row r="767" spans="1:4">
@@ -11026,13 +11029,10 @@
         <v>303</v>
       </c>
       <c r="B767" t="s">
-        <v>310</v>
+        <v>111</v>
       </c>
       <c r="C767">
         <v>0</v>
-      </c>
-      <c r="D767">
-        <v>1</v>
       </c>
     </row>
     <row r="768" spans="1:4">
@@ -11040,7 +11040,7 @@
         <v>303</v>
       </c>
       <c r="B768" t="s">
-        <v>18</v>
+        <v>310</v>
       </c>
       <c r="C768">
         <v>0</v>
@@ -11054,7 +11054,7 @@
         <v>303</v>
       </c>
       <c r="B769" t="s">
-        <v>311</v>
+        <v>18</v>
       </c>
       <c r="C769">
         <v>0</v>
@@ -11068,7 +11068,7 @@
         <v>303</v>
       </c>
       <c r="B770" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C770">
         <v>0</v>
@@ -11082,10 +11082,13 @@
         <v>303</v>
       </c>
       <c r="B771" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C771">
         <v>0</v>
+      </c>
+      <c r="D771">
+        <v>1</v>
       </c>
     </row>
     <row r="772" spans="1:4">
@@ -11093,13 +11096,10 @@
         <v>303</v>
       </c>
       <c r="B772" t="s">
-        <v>298</v>
+        <v>313</v>
       </c>
       <c r="C772">
         <v>0</v>
-      </c>
-      <c r="D772">
-        <v>1</v>
       </c>
     </row>
     <row r="773" spans="1:4">
@@ -11107,10 +11107,13 @@
         <v>303</v>
       </c>
       <c r="B773" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="C773">
         <v>0</v>
+      </c>
+      <c r="D773">
+        <v>1</v>
       </c>
     </row>
     <row r="774" spans="1:4">
@@ -11118,7 +11121,7 @@
         <v>303</v>
       </c>
       <c r="B774" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C774">
         <v>0</v>
@@ -11129,7 +11132,7 @@
         <v>303</v>
       </c>
       <c r="B775" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C775">
         <v>0</v>
@@ -11140,7 +11143,7 @@
         <v>303</v>
       </c>
       <c r="B776" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C776">
         <v>0</v>
@@ -11151,7 +11154,7 @@
         <v>303</v>
       </c>
       <c r="B777" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C777">
         <v>0</v>
@@ -11162,7 +11165,7 @@
         <v>303</v>
       </c>
       <c r="B778" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C778">
         <v>0</v>
@@ -11173,7 +11176,7 @@
         <v>303</v>
       </c>
       <c r="B779" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C779">
         <v>0</v>
@@ -11184,7 +11187,7 @@
         <v>303</v>
       </c>
       <c r="B780" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C780">
         <v>0</v>
@@ -11195,7 +11198,7 @@
         <v>303</v>
       </c>
       <c r="B781" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C781">
         <v>0</v>
@@ -11206,7 +11209,7 @@
         <v>303</v>
       </c>
       <c r="B782" t="s">
-        <v>50</v>
+        <v>322</v>
       </c>
       <c r="C782">
         <v>0</v>
@@ -11217,7 +11220,7 @@
         <v>303</v>
       </c>
       <c r="B783" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C783">
         <v>0</v>
@@ -11228,7 +11231,7 @@
         <v>303</v>
       </c>
       <c r="B784" t="s">
-        <v>323</v>
+        <v>51</v>
       </c>
       <c r="C784">
         <v>0</v>
@@ -11239,53 +11242,53 @@
         <v>303</v>
       </c>
       <c r="B785" t="s">
+        <v>323</v>
+      </c>
+      <c r="C785">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="786" spans="1:4">
+      <c r="A786" t="s">
+        <v>303</v>
+      </c>
+      <c r="B786" t="s">
         <v>324</v>
       </c>
-      <c r="C785">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="786" spans="1:4">
-      <c r="A786" s="1" t="s">
+      <c r="C786">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="787" spans="1:4">
+      <c r="A787" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="B786" s="1" t="s">
+      <c r="B787" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="C786" s="1">
-        <v>0</v>
-      </c>
-      <c r="D786" s="1"/>
-    </row>
-    <row r="787" spans="1:4">
-      <c r="A787" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="B787" s="2" t="s">
-        <v>225</v>
-      </c>
       <c r="C787" s="1">
         <v>0</v>
       </c>
-      <c r="D787" s="2"/>
+      <c r="D787" s="1"/>
     </row>
     <row r="788" spans="1:4">
       <c r="A788" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="B788" t="s">
-        <v>140</v>
+      <c r="B788" s="2" t="s">
+        <v>225</v>
       </c>
       <c r="C788" s="1">
         <v>0</v>
       </c>
+      <c r="D788" s="2"/>
     </row>
     <row r="789" spans="1:4">
       <c r="A789" s="2" t="s">
         <v>404</v>
       </c>
       <c r="B789" t="s">
-        <v>405</v>
+        <v>140</v>
       </c>
       <c r="C789" s="1">
         <v>0</v>
@@ -11296,7 +11299,7 @@
         <v>404</v>
       </c>
       <c r="B790" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C790" s="1">
         <v>0</v>
@@ -11307,7 +11310,7 @@
         <v>404</v>
       </c>
       <c r="B791" t="s">
-        <v>5</v>
+        <v>406</v>
       </c>
       <c r="C791" s="1">
         <v>0</v>
@@ -11318,7 +11321,7 @@
         <v>404</v>
       </c>
       <c r="B792" t="s">
-        <v>407</v>
+        <v>5</v>
       </c>
       <c r="C792" s="1">
         <v>0</v>
@@ -11329,7 +11332,7 @@
         <v>404</v>
       </c>
       <c r="B793" t="s">
-        <v>388</v>
+        <v>407</v>
       </c>
       <c r="C793" s="1">
         <v>0</v>
@@ -11340,9 +11343,20 @@
         <v>404</v>
       </c>
       <c r="B794" t="s">
+        <v>388</v>
+      </c>
+      <c r="C794" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="795" spans="1:4">
+      <c r="A795" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="B795" t="s">
         <v>9</v>
       </c>
-      <c r="C794" s="1">
+      <c r="C795" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>